<commit_message>
Added bi weekly lockdowns and some runs to compare against benchmarks
</commit_message>
<xml_diff>
--- a/benchmarks/linearization_heuristic+Benchmarks_results_90_days.xlsx
+++ b/benchmarks/linearization_heuristic+Benchmarks_results_90_days.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/afs/ir.stanford.edu/users/x/w/xwarnes/GitHub/covid-optimization/benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80215E0A-98DC-5A47-A83F-5A5FAF6B1494}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3D66AD-D2BC-8E4B-B4B2-205C3793FC0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21000" yWindow="3280" windowWidth="32780" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23660" yWindow="5600" windowWidth="32780" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="29">
   <si>
     <t>deaths</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>linearization_heuristic_first_principles</t>
+  </si>
+  <si>
+    <t>linearization_heuristic -- weekly testing -- biweekly lock</t>
+  </si>
+  <si>
+    <t>linearization_heuristic_Prop_Bouncing -- weekly testing -- biweekly lock</t>
   </si>
 </sst>
 </file>
@@ -471,17 +477,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J171"/>
+  <dimension ref="A1:J179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G175" sqref="G175"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="G184" sqref="G184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
     <col min="7" max="7" width="25.5" customWidth="1"/>
     <col min="8" max="8" width="26.5" customWidth="1"/>
   </cols>
@@ -579,7 +586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -611,30 +618,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
       <c r="B5">
-        <v>61135.70941644776</v>
+        <v>75931.287596461203</v>
       </c>
       <c r="C5">
         <v>0.5</v>
       </c>
       <c r="D5">
-        <v>45374351407.829048</v>
+        <v>45475775742.996201</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F5">
         <v>2000</v>
       </c>
       <c r="G5">
-        <v>37878629676.637573</v>
+        <v>38907652232.122704</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="I5">
         <v>30000</v>
@@ -707,7 +712,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>32</v>
       </c>
@@ -739,7 +744,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>31</v>
       </c>
@@ -1091,50 +1096,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>61135.70941644776</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>45374351407.829048</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>2000</v>
+      </c>
+      <c r="G20">
+        <v>37878629676.637573</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20">
+        <v>30000</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>131</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>76493.02222308013</v>
       </c>
-      <c r="C20">
-        <v>0.5</v>
-      </c>
-      <c r="D20">
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
         <v>45692670299.384941</v>
-      </c>
-      <c r="E20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20">
-        <v>2000</v>
-      </c>
-      <c r="G20">
-        <v>36936315888.299469</v>
-      </c>
-      <c r="H20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20">
-        <v>30000</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>132</v>
-      </c>
-      <c r="B21">
-        <v>76468.966708554668</v>
-      </c>
-      <c r="C21">
-        <v>0.5</v>
-      </c>
-      <c r="D21">
-        <v>45681872443.045227</v>
       </c>
       <c r="E21" t="s">
         <v>24</v>
@@ -1143,10 +1148,10 @@
         <v>2000</v>
       </c>
       <c r="G21">
-        <v>36900645417.491951</v>
+        <v>36936315888.299469</v>
       </c>
       <c r="H21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I21">
         <v>30000</v>
@@ -1155,18 +1160,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B22">
-        <v>89519.889499620855</v>
+        <v>76468.966708554668</v>
       </c>
       <c r="C22">
         <v>0.5</v>
       </c>
       <c r="D22">
-        <v>45692079294.099579</v>
+        <v>45681872443.045227</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
@@ -1175,10 +1180,10 @@
         <v>2000</v>
       </c>
       <c r="G22">
-        <v>36889127901.80983</v>
+        <v>36900645417.491951</v>
       </c>
       <c r="H22" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I22">
         <v>30000</v>
@@ -1187,18 +1192,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B23">
-        <v>104513.00660286591</v>
+        <v>89519.889499620855</v>
       </c>
       <c r="C23">
         <v>0.5</v>
       </c>
       <c r="D23">
-        <v>45691116442.457909</v>
+        <v>45692079294.099579</v>
       </c>
       <c r="E23" t="s">
         <v>24</v>
@@ -1207,10 +1212,10 @@
         <v>2000</v>
       </c>
       <c r="G23">
-        <v>36827225563.914177</v>
+        <v>36889127901.80983</v>
       </c>
       <c r="H23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I23">
         <v>30000</v>
@@ -1219,18 +1224,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B24">
-        <v>76853.387521036348</v>
+        <v>104513.00660286591</v>
       </c>
       <c r="C24">
         <v>0.5</v>
       </c>
       <c r="D24">
-        <v>45630534694.182037</v>
+        <v>45691116442.457909</v>
       </c>
       <c r="E24" t="s">
         <v>24</v>
@@ -1239,10 +1244,10 @@
         <v>2000</v>
       </c>
       <c r="G24">
-        <v>36639180376.718033</v>
+        <v>36827225563.914177</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I24">
         <v>30000</v>
@@ -1251,18 +1256,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B25">
-        <v>82759.777568824735</v>
+        <v>76853.387521036348</v>
       </c>
       <c r="C25">
         <v>0.5</v>
       </c>
       <c r="D25">
-        <v>45624202826.455658</v>
+        <v>45630534694.182037</v>
       </c>
       <c r="E25" t="s">
         <v>24</v>
@@ -1271,10 +1276,10 @@
         <v>2000</v>
       </c>
       <c r="G25">
-        <v>36547894754.880836</v>
+        <v>36639180376.718033</v>
       </c>
       <c r="H25" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I25">
         <v>30000</v>
@@ -1283,18 +1288,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B26">
-        <v>84501.197139652882</v>
+        <v>82759.777568824735</v>
       </c>
       <c r="C26">
         <v>0.5</v>
       </c>
       <c r="D26">
-        <v>45611555088.877579</v>
+        <v>45624202826.455658</v>
       </c>
       <c r="E26" t="s">
         <v>24</v>
@@ -1303,10 +1308,10 @@
         <v>2000</v>
       </c>
       <c r="G26">
-        <v>36444544761.734222</v>
+        <v>36547894754.880836</v>
       </c>
       <c r="H26" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I26">
         <v>30000</v>
@@ -1315,18 +1320,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B27">
-        <v>77635.159985174396</v>
+        <v>84501.197139652882</v>
       </c>
       <c r="C27">
         <v>0.5</v>
       </c>
       <c r="D27">
-        <v>45552330647.758202</v>
+        <v>45611555088.877579</v>
       </c>
       <c r="E27" t="s">
         <v>24</v>
@@ -1335,10 +1340,10 @@
         <v>2000</v>
       </c>
       <c r="G27">
-        <v>36143251421.835648</v>
+        <v>36444544761.734222</v>
       </c>
       <c r="H27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I27">
         <v>30000</v>
@@ -1347,18 +1352,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28">
-        <v>77972.636944767553</v>
+        <v>77635.159985174396</v>
       </c>
       <c r="C28">
         <v>0.5</v>
       </c>
       <c r="D28">
-        <v>45517080550.665993</v>
+        <v>45552330647.758202</v>
       </c>
       <c r="E28" t="s">
         <v>24</v>
@@ -1367,10 +1372,10 @@
         <v>2000</v>
       </c>
       <c r="G28">
-        <v>36060638338.974571</v>
+        <v>36143251421.835648</v>
       </c>
       <c r="H28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I28">
         <v>30000</v>
@@ -1379,18 +1384,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B29">
-        <v>80292.148994584961</v>
+        <v>77972.636944767553</v>
       </c>
       <c r="C29">
         <v>0.5</v>
       </c>
       <c r="D29">
-        <v>45500943700.806664</v>
+        <v>45517080550.665993</v>
       </c>
       <c r="E29" t="s">
         <v>24</v>
@@ -1399,10 +1404,10 @@
         <v>2000</v>
       </c>
       <c r="G29">
-        <v>35945493931.87793</v>
+        <v>36060638338.974571</v>
       </c>
       <c r="H29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I29">
         <v>30000</v>
@@ -1731,7 +1736,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>34</v>
       </c>
@@ -1763,7 +1768,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>33</v>
       </c>
@@ -1795,7 +1800,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>35</v>
       </c>
@@ -1827,7 +1832,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>36</v>
       </c>
@@ -1859,7 +1864,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>30</v>
       </c>
@@ -1891,7 +1896,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>74</v>
       </c>
@@ -1923,7 +1928,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>75</v>
       </c>
@@ -1955,7 +1960,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>72</v>
       </c>
@@ -1987,7 +1992,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>73</v>
       </c>
@@ -2019,7 +2024,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>71</v>
       </c>
@@ -2371,50 +2376,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
+        <v>136</v>
+      </c>
+      <c r="B60">
+        <v>80292.148994584961</v>
+      </c>
+      <c r="C60">
+        <v>0.5</v>
+      </c>
+      <c r="D60">
+        <v>45500943700.806664</v>
+      </c>
+      <c r="E60" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60">
+        <v>2000</v>
+      </c>
+      <c r="G60">
+        <v>35945493931.87793</v>
+      </c>
+      <c r="H60" t="s">
+        <v>18</v>
+      </c>
+      <c r="I60">
+        <v>30000</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>15</v>
       </c>
-      <c r="B60">
+      <c r="B61">
         <v>24063.7167217729</v>
       </c>
-      <c r="C60">
-        <v>0.5</v>
-      </c>
-      <c r="D60">
+      <c r="C61">
+        <v>0.5</v>
+      </c>
+      <c r="D61">
         <v>26038427122.019909</v>
-      </c>
-      <c r="E60" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60">
-        <v>2000</v>
-      </c>
-      <c r="G60">
-        <v>22599840289.700722</v>
-      </c>
-      <c r="H60" t="s">
-        <v>17</v>
-      </c>
-      <c r="I60">
-        <v>30000</v>
-      </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <v>14</v>
-      </c>
-      <c r="B61">
-        <v>23903.872474536049</v>
-      </c>
-      <c r="C61">
-        <v>0.5</v>
-      </c>
-      <c r="D61">
-        <v>25943991993.935848</v>
       </c>
       <c r="E61" t="s">
         <v>11</v>
@@ -2423,10 +2428,10 @@
         <v>2000</v>
       </c>
       <c r="G61">
-        <v>22517654927.29821</v>
+        <v>22599840289.700722</v>
       </c>
       <c r="H61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I61">
         <v>30000</v>
@@ -2435,18 +2440,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B62">
-        <v>24982.28481735395</v>
+        <v>23903.872474536049</v>
       </c>
       <c r="C62">
         <v>0.5</v>
       </c>
       <c r="D62">
-        <v>25907854092.22858</v>
+        <v>25943991993.935848</v>
       </c>
       <c r="E62" t="s">
         <v>11</v>
@@ -2455,10 +2460,10 @@
         <v>2000</v>
       </c>
       <c r="G62">
-        <v>22428154763.56657</v>
+        <v>22517654927.29821</v>
       </c>
       <c r="H62" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I62">
         <v>30000</v>
@@ -2467,18 +2472,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B63">
-        <v>23769.053028574359</v>
+        <v>24982.28481735395</v>
       </c>
       <c r="C63">
         <v>0.5</v>
       </c>
       <c r="D63">
-        <v>25603298136.0681</v>
+        <v>25907854092.22858</v>
       </c>
       <c r="E63" t="s">
         <v>11</v>
@@ -2487,10 +2492,10 @@
         <v>2000</v>
       </c>
       <c r="G63">
-        <v>22326562779.892719</v>
+        <v>22428154763.56657</v>
       </c>
       <c r="H63" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I63">
         <v>30000</v>
@@ -2499,18 +2504,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B64">
-        <v>25443.990488585241</v>
+        <v>23769.053028574359</v>
       </c>
       <c r="C64">
         <v>0.5</v>
       </c>
       <c r="D64">
-        <v>25681265238.053619</v>
+        <v>25603298136.0681</v>
       </c>
       <c r="E64" t="s">
         <v>11</v>
@@ -2519,10 +2524,10 @@
         <v>2000</v>
       </c>
       <c r="G64">
-        <v>22322413506.488419</v>
+        <v>22326562779.892719</v>
       </c>
       <c r="H64" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I64">
         <v>30000</v>
@@ -2531,18 +2536,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B65">
-        <v>23411.004095767919</v>
+        <v>25443.990488585241</v>
       </c>
       <c r="C65">
         <v>0.5</v>
       </c>
       <c r="D65">
-        <v>25382547065.410648</v>
+        <v>25681265238.053619</v>
       </c>
       <c r="E65" t="s">
         <v>11</v>
@@ -2551,10 +2556,10 @@
         <v>2000</v>
       </c>
       <c r="G65">
-        <v>22207206899.128399</v>
+        <v>22322413506.488419</v>
       </c>
       <c r="H65" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I65">
         <v>30000</v>
@@ -2563,18 +2568,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B66">
-        <v>23489.058471749791</v>
+        <v>23411.004095767919</v>
       </c>
       <c r="C66">
         <v>0.5</v>
       </c>
       <c r="D66">
-        <v>25325388674.277729</v>
+        <v>25382547065.410648</v>
       </c>
       <c r="E66" t="s">
         <v>11</v>
@@ -2583,10 +2588,10 @@
         <v>2000</v>
       </c>
       <c r="G66">
-        <v>22144092284.99855</v>
+        <v>22207206899.128399</v>
       </c>
       <c r="H66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I66">
         <v>30000</v>
@@ -2595,18 +2600,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B67">
-        <v>26116.61664329467</v>
+        <v>23489.058471749791</v>
       </c>
       <c r="C67">
         <v>0.5</v>
       </c>
       <c r="D67">
-        <v>25476088775.11676</v>
+        <v>25325388674.277729</v>
       </c>
       <c r="E67" t="s">
         <v>11</v>
@@ -2615,10 +2620,10 @@
         <v>2000</v>
       </c>
       <c r="G67">
-        <v>22077699853.435921</v>
+        <v>22144092284.99855</v>
       </c>
       <c r="H67" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I67">
         <v>30000</v>
@@ -2627,18 +2632,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B68">
-        <v>27065.314384988142</v>
+        <v>26116.61664329467</v>
       </c>
       <c r="C68">
         <v>0.5</v>
       </c>
       <c r="D68">
-        <v>25324156658.592831</v>
+        <v>25476088775.11676</v>
       </c>
       <c r="E68" t="s">
         <v>11</v>
@@ -2647,10 +2652,10 @@
         <v>2000</v>
       </c>
       <c r="G68">
-        <v>21991799433.5061</v>
+        <v>22077699853.435921</v>
       </c>
       <c r="H68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I68">
         <v>30000</v>
@@ -2659,18 +2664,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B69">
-        <v>30023.950497196631</v>
+        <v>27065.314384988142</v>
       </c>
       <c r="C69">
         <v>0.5</v>
       </c>
       <c r="D69">
-        <v>25323638096.75692</v>
+        <v>25324156658.592831</v>
       </c>
       <c r="E69" t="s">
         <v>11</v>
@@ -2679,10 +2684,10 @@
         <v>2000</v>
       </c>
       <c r="G69">
-        <v>21918749047.324459</v>
+        <v>21991799433.5061</v>
       </c>
       <c r="H69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I69">
         <v>30000</v>
@@ -3011,7 +3016,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>37</v>
       </c>
@@ -3043,7 +3048,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>76</v>
       </c>
@@ -3075,7 +3080,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>38</v>
       </c>
@@ -3107,7 +3112,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>70</v>
       </c>
@@ -3139,7 +3144,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>77</v>
       </c>
@@ -3171,7 +3176,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>78</v>
       </c>
@@ -3203,7 +3208,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>39</v>
       </c>
@@ -3235,7 +3240,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>114</v>
       </c>
@@ -3267,7 +3272,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>115</v>
       </c>
@@ -3299,7 +3304,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>79</v>
       </c>
@@ -3651,50 +3656,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
+        <v>19</v>
+      </c>
+      <c r="B100">
+        <v>30023.950497196631</v>
+      </c>
+      <c r="C100">
+        <v>0.5</v>
+      </c>
+      <c r="D100">
+        <v>25323638096.75692</v>
+      </c>
+      <c r="E100" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100">
+        <v>2000</v>
+      </c>
+      <c r="G100">
+        <v>21918749047.324459</v>
+      </c>
+      <c r="H100" t="s">
+        <v>21</v>
+      </c>
+      <c r="I100">
+        <v>30000</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
         <v>55</v>
       </c>
-      <c r="B100">
+      <c r="B101">
         <v>21361.217460565149</v>
       </c>
-      <c r="C100">
-        <v>0.5</v>
-      </c>
-      <c r="D100">
+      <c r="C101">
+        <v>0.5</v>
+      </c>
+      <c r="D101">
         <v>20267332536.053719</v>
-      </c>
-      <c r="E100" t="s">
-        <v>22</v>
-      </c>
-      <c r="F100">
-        <v>2000</v>
-      </c>
-      <c r="G100">
-        <v>17202926625.051601</v>
-      </c>
-      <c r="H100" t="s">
-        <v>17</v>
-      </c>
-      <c r="I100">
-        <v>30000</v>
-      </c>
-      <c r="J100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A101" s="1">
-        <v>54</v>
-      </c>
-      <c r="B101">
-        <v>21171.225055369079</v>
-      </c>
-      <c r="C101">
-        <v>0.5</v>
-      </c>
-      <c r="D101">
-        <v>20101614053.26363</v>
       </c>
       <c r="E101" t="s">
         <v>22</v>
@@ -3703,10 +3708,10 @@
         <v>2000</v>
       </c>
       <c r="G101">
-        <v>17052464163.29565</v>
+        <v>17202926625.051601</v>
       </c>
       <c r="H101" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I101">
         <v>30000</v>
@@ -3715,18 +3720,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B102">
-        <v>22108.275274640881</v>
+        <v>21171.225055369079</v>
       </c>
       <c r="C102">
         <v>0.5</v>
       </c>
       <c r="D102">
-        <v>20035862225.05909</v>
+        <v>20101614053.26363</v>
       </c>
       <c r="E102" t="s">
         <v>22</v>
@@ -3735,10 +3740,10 @@
         <v>2000</v>
       </c>
       <c r="G102">
-        <v>16940439132.83099</v>
+        <v>17052464163.29565</v>
       </c>
       <c r="H102" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I102">
         <v>30000</v>
@@ -3747,18 +3752,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B103">
-        <v>22536.048287109341</v>
+        <v>22108.275274640881</v>
       </c>
       <c r="C103">
         <v>0.5</v>
       </c>
       <c r="D103">
-        <v>19661964823.227219</v>
+        <v>20035862225.05909</v>
       </c>
       <c r="E103" t="s">
         <v>22</v>
@@ -3767,10 +3772,10 @@
         <v>2000</v>
       </c>
       <c r="G103">
-        <v>16670125367.667021</v>
+        <v>16940439132.83099</v>
       </c>
       <c r="H103" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I103">
         <v>30000</v>
@@ -3779,18 +3784,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B104">
-        <v>21005.698396268748</v>
+        <v>22536.048287109341</v>
       </c>
       <c r="C104">
         <v>0.5</v>
       </c>
       <c r="D104">
-        <v>19498702822.720089</v>
+        <v>19661964823.227219</v>
       </c>
       <c r="E104" t="s">
         <v>22</v>
@@ -3799,10 +3804,10 @@
         <v>2000</v>
       </c>
       <c r="G104">
-        <v>16586731835.19878</v>
+        <v>16670125367.667021</v>
       </c>
       <c r="H104" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I104">
         <v>30000</v>
@@ -3811,18 +3816,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B105">
-        <v>20684.83304849601</v>
+        <v>21005.698396268748</v>
       </c>
       <c r="C105">
         <v>0.5</v>
       </c>
       <c r="D105">
-        <v>19121303093.281639</v>
+        <v>19498702822.720089</v>
       </c>
       <c r="E105" t="s">
         <v>22</v>
@@ -3831,10 +3836,10 @@
         <v>2000</v>
       </c>
       <c r="G105">
-        <v>16300471876.809629</v>
+        <v>16586731835.19878</v>
       </c>
       <c r="H105" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I105">
         <v>30000</v>
@@ -3843,18 +3848,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B106">
-        <v>23125.87847440011</v>
+        <v>20684.83304849601</v>
       </c>
       <c r="C106">
         <v>0.5</v>
       </c>
       <c r="D106">
-        <v>19288153411.084431</v>
+        <v>19121303093.281639</v>
       </c>
       <c r="E106" t="s">
         <v>22</v>
@@ -3863,10 +3868,10 @@
         <v>2000</v>
       </c>
       <c r="G106">
-        <v>16260861984.28718</v>
+        <v>16300471876.809629</v>
       </c>
       <c r="H106" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I106">
         <v>30000</v>
@@ -3875,18 +3880,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B107">
-        <v>20750.62089947232</v>
+        <v>23125.87847440011</v>
       </c>
       <c r="C107">
         <v>0.5</v>
       </c>
       <c r="D107">
-        <v>19023392633.209332</v>
+        <v>19288153411.084431</v>
       </c>
       <c r="E107" t="s">
         <v>22</v>
@@ -3895,10 +3900,10 @@
         <v>2000</v>
       </c>
       <c r="G107">
-        <v>16197422609.60181</v>
+        <v>16260861984.28718</v>
       </c>
       <c r="H107" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I107">
         <v>30000</v>
@@ -3907,18 +3912,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B108">
-        <v>23968.6981179799</v>
+        <v>20750.62089947232</v>
       </c>
       <c r="C108">
         <v>0.5</v>
       </c>
       <c r="D108">
-        <v>19022322726.398029</v>
+        <v>19023392633.209332</v>
       </c>
       <c r="E108" t="s">
         <v>22</v>
@@ -3927,10 +3932,10 @@
         <v>2000</v>
       </c>
       <c r="G108">
-        <v>16049551403.56159</v>
+        <v>16197422609.60181</v>
       </c>
       <c r="H108" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I108">
         <v>30000</v>
@@ -3939,18 +3944,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B109">
-        <v>26529.914723114511</v>
+        <v>23968.6981179799</v>
       </c>
       <c r="C109">
         <v>0.5</v>
       </c>
       <c r="D109">
-        <v>19021961642.033379</v>
+        <v>19022322726.398029</v>
       </c>
       <c r="E109" t="s">
         <v>22</v>
@@ -3959,10 +3964,10 @@
         <v>2000</v>
       </c>
       <c r="G109">
-        <v>15991291357.797029</v>
+        <v>16049551403.56159</v>
       </c>
       <c r="H109" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I109">
         <v>30000</v>
@@ -4291,7 +4296,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>113</v>
       </c>
@@ -4323,7 +4328,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>112</v>
       </c>
@@ -4355,7 +4360,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>111</v>
       </c>
@@ -4387,7 +4392,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>116</v>
       </c>
@@ -4419,7 +4424,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>110</v>
       </c>
@@ -4451,7 +4456,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>117</v>
       </c>
@@ -4483,7 +4488,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>118</v>
       </c>
@@ -4515,7 +4520,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>6</v>
       </c>
@@ -4547,7 +4552,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>119</v>
       </c>
@@ -4579,7 +4584,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>7</v>
       </c>
@@ -4931,50 +4936,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
+        <v>59</v>
+      </c>
+      <c r="B140">
+        <v>26529.914723114511</v>
+      </c>
+      <c r="C140">
+        <v>0.5</v>
+      </c>
+      <c r="D140">
+        <v>19021961642.033379</v>
+      </c>
+      <c r="E140" t="s">
+        <v>22</v>
+      </c>
+      <c r="F140">
+        <v>2000</v>
+      </c>
+      <c r="G140">
+        <v>15991291357.797029</v>
+      </c>
+      <c r="H140" t="s">
+        <v>21</v>
+      </c>
+      <c r="I140">
+        <v>30000</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
         <v>95</v>
       </c>
-      <c r="B140">
+      <c r="B141">
         <v>20822.087903888802</v>
       </c>
-      <c r="C140">
-        <v>0.5</v>
-      </c>
-      <c r="D140">
+      <c r="C141">
+        <v>0.5</v>
+      </c>
+      <c r="D141">
         <v>13004979207.748819</v>
-      </c>
-      <c r="E140" t="s">
-        <v>23</v>
-      </c>
-      <c r="F140">
-        <v>2000</v>
-      </c>
-      <c r="G140">
-        <v>10024771699.23962</v>
-      </c>
-      <c r="H140" t="s">
-        <v>17</v>
-      </c>
-      <c r="I140">
-        <v>30000</v>
-      </c>
-      <c r="J140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A141" s="1">
-        <v>94</v>
-      </c>
-      <c r="B141">
-        <v>20626.669741520309</v>
-      </c>
-      <c r="C141">
-        <v>0.5</v>
-      </c>
-      <c r="D141">
-        <v>12793685173.17964</v>
       </c>
       <c r="E141" t="s">
         <v>23</v>
@@ -4983,10 +4988,10 @@
         <v>2000</v>
       </c>
       <c r="G141">
-        <v>9828962959.1646347</v>
+        <v>10024771699.23962</v>
       </c>
       <c r="H141" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I141">
         <v>30000</v>
@@ -4995,18 +5000,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B142">
-        <v>21534.299247355699</v>
+        <v>20626.669741520309</v>
       </c>
       <c r="C142">
         <v>0.5</v>
       </c>
       <c r="D142">
-        <v>12710451017.524389</v>
+        <v>12793685173.17964</v>
       </c>
       <c r="E142" t="s">
         <v>23</v>
@@ -5015,10 +5020,10 @@
         <v>2000</v>
       </c>
       <c r="G142">
-        <v>9701025724.949482</v>
+        <v>9828962959.1646347</v>
       </c>
       <c r="H142" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I142">
         <v>30000</v>
@@ -5027,18 +5032,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B143">
-        <v>21949.020584726932</v>
+        <v>21534.299247355699</v>
       </c>
       <c r="C143">
         <v>0.5</v>
       </c>
       <c r="D143">
-        <v>12230213709.06971</v>
+        <v>12710451017.524389</v>
       </c>
       <c r="E143" t="s">
         <v>23</v>
@@ -5047,10 +5052,10 @@
         <v>2000</v>
       </c>
       <c r="G143">
-        <v>9321175947.6178722</v>
+        <v>9701025724.949482</v>
       </c>
       <c r="H143" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I143">
         <v>30000</v>
@@ -5059,18 +5064,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B144">
-        <v>20464.017846168768</v>
+        <v>21949.020584726932</v>
       </c>
       <c r="C144">
         <v>0.5</v>
       </c>
       <c r="D144">
-        <v>12020589552.05784</v>
+        <v>12230213709.06971</v>
       </c>
       <c r="E144" t="s">
         <v>23</v>
@@ -5079,10 +5084,10 @@
         <v>2000</v>
       </c>
       <c r="G144">
-        <v>9189205396.1966839</v>
+        <v>9321175947.6178722</v>
       </c>
       <c r="H144" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I144">
         <v>30000</v>
@@ -5091,18 +5096,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B145">
-        <v>22530.550530083208</v>
+        <v>20464.017846168768</v>
       </c>
       <c r="C145">
         <v>0.5</v>
       </c>
       <c r="D145">
-        <v>11755267387.44474</v>
+        <v>12020589552.05784</v>
       </c>
       <c r="E145" t="s">
         <v>23</v>
@@ -5111,10 +5116,10 @@
         <v>2000</v>
       </c>
       <c r="G145">
-        <v>8811015134.6077042</v>
+        <v>9189205396.1966839</v>
       </c>
       <c r="H145" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I145">
         <v>30000</v>
@@ -5123,18 +5128,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B146">
-        <v>20141.275508210809</v>
+        <v>22530.550530083208</v>
       </c>
       <c r="C146">
         <v>0.5</v>
       </c>
       <c r="D146">
-        <v>11538656672.076599</v>
+        <v>11755267387.44474</v>
       </c>
       <c r="E146" t="s">
         <v>23</v>
@@ -5143,10 +5148,10 @@
         <v>2000</v>
       </c>
       <c r="G146">
-        <v>8797459285.4957466</v>
+        <v>8811015134.6077042</v>
       </c>
       <c r="H146" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I146">
         <v>30000</v>
@@ -5155,18 +5160,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B147">
-        <v>20204.21675520407</v>
+        <v>20141.275508210809</v>
       </c>
       <c r="C147">
         <v>0.5</v>
       </c>
       <c r="D147">
-        <v>11412353729.80073</v>
+        <v>11538656672.076599</v>
       </c>
       <c r="E147" t="s">
         <v>23</v>
@@ -5175,10 +5180,10 @@
         <v>2000</v>
       </c>
       <c r="G147">
-        <v>8666211435.9383888</v>
+        <v>8797459285.4957466</v>
       </c>
       <c r="H147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I147">
         <v>30000</v>
@@ -5187,18 +5192,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B148">
-        <v>23352.711087550659</v>
+        <v>20204.21675520407</v>
       </c>
       <c r="C148">
         <v>0.5</v>
       </c>
       <c r="D148">
-        <v>11411382815.65556</v>
+        <v>11412353729.80073</v>
       </c>
       <c r="E148" t="s">
         <v>23</v>
@@ -5207,10 +5212,10 @@
         <v>2000</v>
       </c>
       <c r="G148">
-        <v>8520063240.3933992</v>
+        <v>8666211435.9383888</v>
       </c>
       <c r="H148" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I148">
         <v>30000</v>
@@ -5219,18 +5224,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B149">
-        <v>25790.727244949579</v>
+        <v>23352.711087550659</v>
       </c>
       <c r="C149">
         <v>0.5</v>
       </c>
       <c r="D149">
-        <v>11411109391.88575</v>
+        <v>11411382815.65556</v>
       </c>
       <c r="E149" t="s">
         <v>23</v>
@@ -5239,10 +5244,10 @@
         <v>2000</v>
       </c>
       <c r="G149">
-        <v>8465090000.3280087</v>
+        <v>8520063240.3933992</v>
       </c>
       <c r="H149" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I149">
         <v>30000</v>
@@ -5571,7 +5576,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="2"/>
       <c r="B160">
         <v>59987.272186896596</v>
@@ -5601,7 +5606,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>151</v>
       </c>
@@ -5633,7 +5638,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>152</v>
       </c>
@@ -5665,7 +5670,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>153</v>
       </c>
@@ -5697,7 +5702,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>154</v>
       </c>
@@ -5729,7 +5734,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>155</v>
       </c>
@@ -5761,7 +5766,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>156</v>
       </c>
@@ -5793,7 +5798,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>150</v>
       </c>
@@ -5825,7 +5830,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>157</v>
       </c>
@@ -5857,7 +5862,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>158</v>
       </c>
@@ -5889,7 +5894,7 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>159</v>
       </c>
@@ -5921,34 +5926,268 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A171" s="2"/>
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>99</v>
+      </c>
       <c r="B171">
-        <v>75931.287596461203</v>
+        <v>25790.727244949579</v>
       </c>
       <c r="C171">
         <v>0.5</v>
       </c>
       <c r="D171">
-        <v>45475775742.996201</v>
+        <v>11411109391.88575</v>
       </c>
       <c r="E171" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F171">
         <v>2000</v>
       </c>
       <c r="G171">
-        <v>38907652232.122704</v>
+        <v>8465090000.3280087</v>
       </c>
       <c r="H171" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I171">
         <v>30000</v>
       </c>
       <c r="J171">
         <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B172">
+        <v>59907.386841751548</v>
+      </c>
+      <c r="C172">
+        <v>0.5</v>
+      </c>
+      <c r="D172">
+        <v>45669430836.814667</v>
+      </c>
+      <c r="E172" t="s">
+        <v>27</v>
+      </c>
+      <c r="F172">
+        <v>2000</v>
+      </c>
+      <c r="G172">
+        <v>39345493500.230591</v>
+      </c>
+      <c r="H172" t="s">
+        <v>9</v>
+      </c>
+      <c r="I172">
+        <v>0</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B173">
+        <v>60452.209425135603</v>
+      </c>
+      <c r="C173">
+        <v>0.5</v>
+      </c>
+      <c r="D173">
+        <v>45661151303.619812</v>
+      </c>
+      <c r="E173" t="s">
+        <v>28</v>
+      </c>
+      <c r="F173">
+        <v>2000</v>
+      </c>
+      <c r="G173">
+        <v>37804064360.125252</v>
+      </c>
+      <c r="H173" t="s">
+        <v>9</v>
+      </c>
+      <c r="I173">
+        <v>0</v>
+      </c>
+      <c r="J173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B174">
+        <v>67445.186139135913</v>
+      </c>
+      <c r="C174">
+        <v>0.5</v>
+      </c>
+      <c r="D174">
+        <v>45634079074.988136</v>
+      </c>
+      <c r="E174" t="s">
+        <v>9</v>
+      </c>
+      <c r="F174">
+        <v>2000</v>
+      </c>
+      <c r="G174">
+        <v>39274548294.962227</v>
+      </c>
+      <c r="H174" t="s">
+        <v>9</v>
+      </c>
+      <c r="I174">
+        <v>30000</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B175">
+        <v>68014.663831286598</v>
+      </c>
+      <c r="C175">
+        <v>0.5</v>
+      </c>
+      <c r="D175">
+        <v>45625055534.595047</v>
+      </c>
+      <c r="E175" t="s">
+        <v>28</v>
+      </c>
+      <c r="F175">
+        <v>2000</v>
+      </c>
+      <c r="G175">
+        <v>37656437856.134041</v>
+      </c>
+      <c r="H175" t="s">
+        <v>9</v>
+      </c>
+      <c r="I175">
+        <v>30000</v>
+      </c>
+      <c r="J175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B176">
+        <v>53903.196729560907</v>
+      </c>
+      <c r="C176">
+        <v>0.5</v>
+      </c>
+      <c r="D176">
+        <v>36152247074.781609</v>
+      </c>
+      <c r="E176" t="s">
+        <v>27</v>
+      </c>
+      <c r="F176">
+        <v>2000</v>
+      </c>
+      <c r="G176">
+        <v>-29941568211.32774</v>
+      </c>
+      <c r="H176" t="s">
+        <v>9</v>
+      </c>
+      <c r="I176">
+        <v>0</v>
+      </c>
+      <c r="J176">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B177">
+        <v>54410.325563740516</v>
+      </c>
+      <c r="C177">
+        <v>0.5</v>
+      </c>
+      <c r="D177">
+        <v>36142898870.665154</v>
+      </c>
+      <c r="E177" t="s">
+        <v>28</v>
+      </c>
+      <c r="F177">
+        <v>2000</v>
+      </c>
+      <c r="G177">
+        <v>-31624764918.147991</v>
+      </c>
+      <c r="H177" t="s">
+        <v>9</v>
+      </c>
+      <c r="I177">
+        <v>0</v>
+      </c>
+      <c r="J177">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="178" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B178">
+        <v>52316.086802824248</v>
+      </c>
+      <c r="C178">
+        <v>0.5</v>
+      </c>
+      <c r="D178">
+        <v>33833532056.768509</v>
+      </c>
+      <c r="E178" t="s">
+        <v>27</v>
+      </c>
+      <c r="F178">
+        <v>2000</v>
+      </c>
+      <c r="G178">
+        <v>-30318561389.1497</v>
+      </c>
+      <c r="H178" t="s">
+        <v>9</v>
+      </c>
+      <c r="I178">
+        <v>30000</v>
+      </c>
+      <c r="J178">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B179">
+        <v>52818.955692821633</v>
+      </c>
+      <c r="C179">
+        <v>0.5</v>
+      </c>
+      <c r="D179">
+        <v>33824347003.661751</v>
+      </c>
+      <c r="E179" t="s">
+        <v>28</v>
+      </c>
+      <c r="F179">
+        <v>2000</v>
+      </c>
+      <c r="G179">
+        <v>-31979931245.781521</v>
+      </c>
+      <c r="H179" t="s">
+        <v>9</v>
+      </c>
+      <c r="I179">
+        <v>30000</v>
+      </c>
+      <c r="J179">
+        <v>1115970.8999999999</v>
       </c>
     </row>
   </sheetData>
@@ -5960,7 +6199,7 @@
     </filterColumn>
     <filterColumn colId="9">
       <filters>
-        <filter val="0"/>
+        <filter val="1115970.9"/>
       </filters>
     </filterColumn>
     <sortState ref="A4:J171">

</xml_diff>

<commit_message>
Added run of heuristic with random initial uhat
</commit_message>
<xml_diff>
--- a/benchmarks/linearization_heuristic+Benchmarks_results_90_days.xlsx
+++ b/benchmarks/linearization_heuristic+Benchmarks_results_90_days.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/afs/ir.stanford.edu/users/x/w/xwarnes/GitHub/covid-optimization/benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3D66AD-D2BC-8E4B-B4B2-205C3793FC0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFC4833-9E72-E948-A4B6-07A14E667ED7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23660" yWindow="5600" windowWidth="32780" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36520" yWindow="4160" windowWidth="32780" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$171</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$203</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="42">
   <si>
     <t>deaths</t>
   </si>
@@ -111,12 +111,51 @@
   <si>
     <t>linearization_heuristic_Prop_Bouncing -- weekly testing -- biweekly lock</t>
   </si>
+  <si>
+    <t>linearization_heuristic -- Open Initial Uhat</t>
+  </si>
+  <si>
+    <t>linearization_heuristic_Prop_Bouncing -- Open initial Uhat</t>
+  </si>
+  <si>
+    <t>linearization_heuristic_Prop_Bouncing -- Open Initial Uhat</t>
+  </si>
+  <si>
+    <t>linearization_heuristic_Prop_Bouncing -- Open Initial Uhat -- weekly-biweekly const</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linearization_heuristic -- Open Initial Uhat -- weekly-biweekly const </t>
+  </si>
+  <si>
+    <t>linearization_heuristic -- daily decisions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linearization_heuristic_Prop_Bouncing -- Open Initial Uhat -- weekly-biweekly const </t>
+  </si>
+  <si>
+    <t>linearization_heuristic -- Random Initial Uhat - weekly-biweekly</t>
+  </si>
+  <si>
+    <t>linearization_heuristic_Prop_Bouncing  -- Random Initial Uhat - weekly-biweekly</t>
+  </si>
+  <si>
+    <t>linearization_heuristic_Prop_Bouncing -- Random Initial Uhat - weekly-biweekly</t>
+  </si>
+  <si>
+    <t>linearization_heuristic -- random initial Uhat - weekly-biweekly -- no Econ values</t>
+  </si>
+  <si>
+    <t>linearization_heuristic_Prop_Bouncing  -- random initial Uhat - weekly-biweekly -- no Econ values</t>
+  </si>
+  <si>
+    <t>linearization_heuristic  -- random initial Uhat - weekly-biweekly -- no Econ values</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +167,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -174,6 +220,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +525,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J179"/>
+  <dimension ref="A1:J203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="G184" sqref="G184"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -488,9 +536,9 @@
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
-    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="57.1640625" customWidth="1"/>
     <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="26.5" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -587,26 +635,24 @@
       </c>
     </row>
     <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4">
-        <v>60537.374334463413</v>
+        <v>53109.090901042597</v>
       </c>
       <c r="C4">
         <v>0.5</v>
       </c>
       <c r="D4">
-        <v>45383149584.349869</v>
+        <v>45052778687.897079</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="F4">
         <v>2000</v>
       </c>
       <c r="G4">
-        <v>39508436511.752388</v>
+        <v>39760638293.259102</v>
       </c>
       <c r="H4" t="s">
         <v>9</v>
@@ -618,34 +664,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>112</v>
+      </c>
       <c r="B5">
-        <v>75931.287596461203</v>
+        <v>20141.275508210809</v>
       </c>
       <c r="C5">
         <v>0.5</v>
       </c>
       <c r="D5">
-        <v>45475775742.996201</v>
+        <v>11538656672.076599</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>2000</v>
       </c>
       <c r="G5">
-        <v>38907652232.122704</v>
+        <v>-13679618070.55022</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="I5">
         <v>30000</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -712,68 +760,64 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>32</v>
-      </c>
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
       <c r="B8">
-        <v>23411.004095767919</v>
+        <v>59907.386841751548</v>
       </c>
       <c r="C8">
         <v>0.5</v>
       </c>
       <c r="D8">
-        <v>25382547065.410648</v>
+        <v>45669430836.814667</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F8">
         <v>2000</v>
       </c>
       <c r="G8">
-        <v>-3918792411.5294151</v>
+        <v>39345493500.230591</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I8">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>31</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
       <c r="B9">
-        <v>23489.058471749791</v>
+        <v>61223.916026000181</v>
       </c>
       <c r="C9">
         <v>0.5</v>
       </c>
       <c r="D9">
-        <v>25325388674.277729</v>
+        <v>45521250505.386726</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="F9">
         <v>2000</v>
       </c>
       <c r="G9">
-        <v>-4069013437.8726912</v>
+        <v>39632764077.428932</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I9">
         <v>30000</v>
       </c>
       <c r="J9">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -1096,318 +1140,310 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="B20">
-        <v>61135.70941644776</v>
+        <v>20204.21675520407</v>
       </c>
       <c r="C20">
         <v>0.5</v>
       </c>
       <c r="D20">
-        <v>45374351407.829048</v>
+        <v>11412353729.80073</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F20">
         <v>2000</v>
       </c>
       <c r="G20">
-        <v>37878629676.637573</v>
+        <v>-13881106520.16177</v>
       </c>
       <c r="H20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I20">
         <v>30000</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>131</v>
+        <v>2</v>
       </c>
       <c r="B21">
-        <v>76493.02222308013</v>
+        <v>60537.374334463413</v>
       </c>
       <c r="C21">
         <v>0.5</v>
       </c>
       <c r="D21">
-        <v>45692670299.384941</v>
+        <v>45383149584.349869</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F21">
         <v>2000</v>
       </c>
       <c r="G21">
-        <v>36936315888.299469</v>
+        <v>39508436511.752388</v>
       </c>
       <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21">
+        <v>30000</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>113</v>
+      </c>
+      <c r="B22">
+        <v>20464.017846168768</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>12020589552.05784</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22">
+        <v>2000</v>
+      </c>
+      <c r="G22">
+        <v>-13648043017.20833</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22">
+        <v>30000</v>
+      </c>
+      <c r="J22">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23">
+        <v>67445.186139135913</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <v>45634079074.988136</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23">
+        <v>2000</v>
+      </c>
+      <c r="G23">
+        <v>39274548294.962227</v>
+      </c>
+      <c r="H23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23">
+        <v>30000</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>114</v>
+      </c>
+      <c r="B24">
+        <v>20626.669741520309</v>
+      </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24">
+        <v>12793685173.17964</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <v>2000</v>
+      </c>
+      <c r="G24">
+        <v>-13189800236.28256</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24">
+        <v>30000</v>
+      </c>
+      <c r="J24">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25">
+        <v>75931.287596461203</v>
+      </c>
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="D25">
+        <v>45475775742.996201</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25">
+        <v>2000</v>
+      </c>
+      <c r="G25">
+        <v>38907652232.122704</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25">
+        <v>30000</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>72</v>
+      </c>
+      <c r="B26">
+        <v>20684.83304849601</v>
+      </c>
+      <c r="C26">
+        <v>0.5</v>
+      </c>
+      <c r="D26">
+        <v>19121303093.281639</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26">
+        <v>2000</v>
+      </c>
+      <c r="G26">
+        <v>-6783199876.6702051</v>
+      </c>
+      <c r="H26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26">
+        <v>30000</v>
+      </c>
+      <c r="J26">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27">
+        <v>53714.221294985298</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>45043998691.606422</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27">
+        <v>2000</v>
+      </c>
+      <c r="G27">
+        <v>38114260182.391129</v>
+      </c>
+      <c r="H27" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <v>30000</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>71</v>
+      </c>
+      <c r="B28">
+        <v>20750.62089947232</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <v>19023392633.209332</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28">
+        <v>2000</v>
+      </c>
+      <c r="G28">
+        <v>-6959666471.141118</v>
+      </c>
+      <c r="H28" t="s">
         <v>13</v>
       </c>
-      <c r="I21">
-        <v>30000</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>132</v>
-      </c>
-      <c r="B22">
-        <v>76468.966708554668</v>
-      </c>
-      <c r="C22">
-        <v>0.5</v>
-      </c>
-      <c r="D22">
-        <v>45681872443.045227</v>
-      </c>
-      <c r="E22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22">
-        <v>2000</v>
-      </c>
-      <c r="G22">
-        <v>36900645417.491951</v>
-      </c>
-      <c r="H22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22">
-        <v>30000</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>138</v>
-      </c>
-      <c r="B23">
-        <v>89519.889499620855</v>
-      </c>
-      <c r="C23">
-        <v>0.5</v>
-      </c>
-      <c r="D23">
-        <v>45692079294.099579</v>
-      </c>
-      <c r="E23" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23">
-        <v>2000</v>
-      </c>
-      <c r="G23">
-        <v>36889127901.80983</v>
-      </c>
-      <c r="H23" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23">
-        <v>30000</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>139</v>
-      </c>
-      <c r="B24">
-        <v>104513.00660286591</v>
-      </c>
-      <c r="C24">
-        <v>0.5</v>
-      </c>
-      <c r="D24">
-        <v>45691116442.457909</v>
-      </c>
-      <c r="E24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24">
-        <v>2000</v>
-      </c>
-      <c r="G24">
-        <v>36827225563.914177</v>
-      </c>
-      <c r="H24" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24">
-        <v>30000</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>133</v>
-      </c>
-      <c r="B25">
-        <v>76853.387521036348</v>
-      </c>
-      <c r="C25">
-        <v>0.5</v>
-      </c>
-      <c r="D25">
-        <v>45630534694.182037</v>
-      </c>
-      <c r="E25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25">
-        <v>2000</v>
-      </c>
-      <c r="G25">
-        <v>36639180376.718033</v>
-      </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25">
-        <v>30000</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>130</v>
-      </c>
-      <c r="B26">
-        <v>82759.777568824735</v>
-      </c>
-      <c r="C26">
-        <v>0.5</v>
-      </c>
-      <c r="D26">
-        <v>45624202826.455658</v>
-      </c>
-      <c r="E26" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26">
-        <v>2000</v>
-      </c>
-      <c r="G26">
-        <v>36547894754.880836</v>
-      </c>
-      <c r="H26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26">
-        <v>30000</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>137</v>
-      </c>
-      <c r="B27">
-        <v>84501.197139652882</v>
-      </c>
-      <c r="C27">
-        <v>0.5</v>
-      </c>
-      <c r="D27">
-        <v>45611555088.877579</v>
-      </c>
-      <c r="E27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27">
-        <v>2000</v>
-      </c>
-      <c r="G27">
-        <v>36444544761.734222</v>
-      </c>
-      <c r="H27" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27">
-        <v>30000</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>134</v>
-      </c>
-      <c r="B28">
-        <v>77635.159985174396</v>
-      </c>
-      <c r="C28">
-        <v>0.5</v>
-      </c>
-      <c r="D28">
-        <v>45552330647.758202</v>
-      </c>
-      <c r="E28" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28">
-        <v>2000</v>
-      </c>
-      <c r="G28">
-        <v>36143251421.835648</v>
-      </c>
-      <c r="H28" t="s">
-        <v>16</v>
-      </c>
       <c r="I28">
         <v>30000</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>135</v>
-      </c>
+      <c r="A29" s="2"/>
       <c r="B29">
-        <v>77972.636944767553</v>
+        <v>61829.892960574907</v>
       </c>
       <c r="C29">
         <v>0.5</v>
       </c>
       <c r="D29">
-        <v>45517080550.665993</v>
+        <v>45512367646.279358</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F29">
         <v>2000</v>
       </c>
       <c r="G29">
-        <v>36060638338.974571</v>
+        <v>37985826093.714371</v>
       </c>
       <c r="H29" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="I29">
         <v>30000</v>
@@ -1736,62 +1772,60 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>34</v>
-      </c>
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
       <c r="B40">
-        <v>23903.872474536049</v>
+        <v>60452.209425135603</v>
       </c>
       <c r="C40">
         <v>0.5</v>
       </c>
       <c r="D40">
-        <v>25943991993.935848</v>
+        <v>45661151303.619812</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F40">
         <v>2000</v>
       </c>
       <c r="G40">
-        <v>-4158371151.5950012</v>
+        <v>37804064360.125252</v>
       </c>
       <c r="H40" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I40">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="B41">
-        <v>23769.053028574359</v>
+        <v>20822.087903888802</v>
       </c>
       <c r="C41">
         <v>0.5</v>
       </c>
       <c r="D41">
-        <v>25603298136.0681</v>
+        <v>13004979207.748819</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F41">
         <v>2000</v>
       </c>
       <c r="G41">
-        <v>-4199008720.5531378</v>
+        <v>-13212072478.742279</v>
       </c>
       <c r="H41" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I41">
         <v>30000</v>
@@ -1800,62 +1834,62 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B42">
-        <v>24063.7167217729</v>
+        <v>61135.70941644776</v>
       </c>
       <c r="C42">
         <v>0.5</v>
       </c>
       <c r="D42">
-        <v>26038427122.019909</v>
+        <v>45374351407.829048</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F42">
         <v>2000</v>
       </c>
       <c r="G42">
-        <v>-4254567317.6411929</v>
+        <v>37878629676.637573</v>
       </c>
       <c r="H42" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="I42">
         <v>30000</v>
       </c>
       <c r="J42">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B43">
-        <v>24982.28481735395</v>
+        <v>21005.698396268748</v>
       </c>
       <c r="C43">
         <v>0.5</v>
       </c>
       <c r="D43">
-        <v>25907854092.22858</v>
+        <v>19498702822.720089</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F43">
         <v>2000</v>
       </c>
       <c r="G43">
-        <v>-5451348108.1122684</v>
+        <v>-6855016309.2138319</v>
       </c>
       <c r="H43" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I43">
         <v>30000</v>
@@ -1864,36 +1898,34 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>30</v>
-      </c>
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
       <c r="B44">
-        <v>25443.990488585241</v>
+        <v>68014.663831286598</v>
       </c>
       <c r="C44">
         <v>0.5</v>
       </c>
       <c r="D44">
-        <v>25681265238.053619</v>
+        <v>45625055534.595047</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F44">
         <v>2000</v>
       </c>
       <c r="G44">
-        <v>-6072339458.6494951</v>
+        <v>37656437856.134041</v>
       </c>
       <c r="H44" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I44">
         <v>30000</v>
       </c>
       <c r="J44">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -1928,50 +1960,50 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="B46">
-        <v>21361.217460565149</v>
+        <v>76493.02222308013</v>
       </c>
       <c r="C46">
         <v>0.5</v>
       </c>
       <c r="D46">
-        <v>20267332536.053719</v>
+        <v>45692670299.384941</v>
       </c>
       <c r="E46" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F46">
         <v>2000</v>
       </c>
       <c r="G46">
-        <v>-6635570449.5109777</v>
+        <v>36936315888.299469</v>
       </c>
       <c r="H46" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I46">
         <v>30000</v>
       </c>
       <c r="J46">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B47">
-        <v>20684.83304849601</v>
+        <v>21361.217460565149</v>
       </c>
       <c r="C47">
         <v>0.5</v>
       </c>
       <c r="D47">
-        <v>19121303093.281639</v>
+        <v>20267332536.053719</v>
       </c>
       <c r="E47" t="s">
         <v>22</v>
@@ -1980,74 +2012,74 @@
         <v>2000</v>
       </c>
       <c r="G47">
-        <v>-6783199876.6702051</v>
+        <v>-6635570449.5109777</v>
       </c>
       <c r="H47" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47">
+        <v>30000</v>
+      </c>
+      <c r="J47">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>132</v>
+      </c>
+      <c r="B48">
+        <v>76468.966708554668</v>
+      </c>
+      <c r="C48">
+        <v>0.5</v>
+      </c>
+      <c r="D48">
+        <v>45681872443.045227</v>
+      </c>
+      <c r="E48" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48">
+        <v>2000</v>
+      </c>
+      <c r="G48">
+        <v>36900645417.491951</v>
+      </c>
+      <c r="H48" t="s">
         <v>14</v>
       </c>
-      <c r="I47">
-        <v>30000</v>
-      </c>
-      <c r="J47">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>73</v>
-      </c>
-      <c r="B48">
-        <v>21005.698396268748</v>
-      </c>
-      <c r="C48">
-        <v>0.5</v>
-      </c>
-      <c r="D48">
-        <v>19498702822.720089</v>
-      </c>
-      <c r="E48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F48">
-        <v>2000</v>
-      </c>
-      <c r="G48">
-        <v>-6855016309.2138319</v>
-      </c>
-      <c r="H48" t="s">
-        <v>15</v>
-      </c>
       <c r="I48">
         <v>30000</v>
       </c>
       <c r="J48">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="B49">
-        <v>20750.62089947232</v>
+        <v>21534.299247355699</v>
       </c>
       <c r="C49">
         <v>0.5</v>
       </c>
       <c r="D49">
-        <v>19023392633.209332</v>
+        <v>12710451017.524389</v>
       </c>
       <c r="E49" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F49">
         <v>2000</v>
       </c>
       <c r="G49">
-        <v>-6959666471.141118</v>
+        <v>-14330625586.991381</v>
       </c>
       <c r="H49" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I49">
         <v>30000</v>
@@ -2378,16 +2410,16 @@
     </row>
     <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B60">
-        <v>80292.148994584961</v>
+        <v>89519.889499620855</v>
       </c>
       <c r="C60">
         <v>0.5</v>
       </c>
       <c r="D60">
-        <v>45500943700.806664</v>
+        <v>45692079294.099579</v>
       </c>
       <c r="E60" t="s">
         <v>24</v>
@@ -2396,10 +2428,10 @@
         <v>2000</v>
       </c>
       <c r="G60">
-        <v>35945493931.87793</v>
+        <v>36889127901.80983</v>
       </c>
       <c r="H60" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I60">
         <v>30000</v>
@@ -2408,62 +2440,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="B61">
-        <v>24063.7167217729</v>
+        <v>21949.020584726932</v>
       </c>
       <c r="C61">
         <v>0.5</v>
       </c>
       <c r="D61">
-        <v>26038427122.019909</v>
+        <v>12230213709.06971</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F61">
         <v>2000</v>
       </c>
       <c r="G61">
-        <v>22599840289.700722</v>
+        <v>-15173292308.438351</v>
       </c>
       <c r="H61" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I61">
         <v>30000</v>
       </c>
       <c r="J61">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>14</v>
+        <v>139</v>
       </c>
       <c r="B62">
-        <v>23903.872474536049</v>
+        <v>104513.00660286591</v>
       </c>
       <c r="C62">
         <v>0.5</v>
       </c>
       <c r="D62">
-        <v>25943991993.935848</v>
+        <v>45691116442.457909</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F62">
         <v>2000</v>
       </c>
       <c r="G62">
-        <v>22517654927.29821</v>
+        <v>36827225563.914177</v>
       </c>
       <c r="H62" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I62">
         <v>30000</v>
@@ -2472,27 +2504,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="B63">
-        <v>24982.28481735395</v>
+        <v>22108.275274640881</v>
       </c>
       <c r="C63">
         <v>0.5</v>
       </c>
       <c r="D63">
-        <v>25907854092.22858</v>
+        <v>20035862225.05909</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F63">
         <v>2000</v>
       </c>
       <c r="G63">
-        <v>22428154763.56657</v>
+        <v>-7731752722.8577595</v>
       </c>
       <c r="H63" t="s">
         <v>18</v>
@@ -2501,30 +2533,30 @@
         <v>30000</v>
       </c>
       <c r="J63">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="B64">
-        <v>23769.053028574359</v>
+        <v>76853.387521036348</v>
       </c>
       <c r="C64">
         <v>0.5</v>
       </c>
       <c r="D64">
-        <v>25603298136.0681</v>
+        <v>45630534694.182037</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F64">
         <v>2000</v>
       </c>
       <c r="G64">
-        <v>22326562779.892719</v>
+        <v>36639180376.718033</v>
       </c>
       <c r="H64" t="s">
         <v>15</v>
@@ -2536,63 +2568,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="B65">
-        <v>25443.990488585241</v>
+        <v>22530.550530083208</v>
       </c>
       <c r="C65">
         <v>0.5</v>
       </c>
       <c r="D65">
-        <v>25681265238.053619</v>
+        <v>11755267387.44474</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F65">
         <v>2000</v>
       </c>
       <c r="G65">
-        <v>22322413506.488419</v>
+        <v>-16332423617.94474</v>
       </c>
       <c r="H65" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I65">
         <v>30000</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
+        <v>130</v>
+      </c>
+      <c r="B66">
+        <v>82759.777568824735</v>
+      </c>
+      <c r="C66">
+        <v>0.5</v>
+      </c>
+      <c r="D66">
+        <v>45624202826.455658</v>
+      </c>
+      <c r="E66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66">
+        <v>2000</v>
+      </c>
+      <c r="G66">
+        <v>36547894754.880836</v>
+      </c>
+      <c r="H66" t="s">
         <v>12</v>
       </c>
-      <c r="B66">
-        <v>23411.004095767919</v>
-      </c>
-      <c r="C66">
-        <v>0.5</v>
-      </c>
-      <c r="D66">
-        <v>25382547065.410648</v>
-      </c>
-      <c r="E66" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66">
-        <v>2000</v>
-      </c>
-      <c r="G66">
-        <v>22207206899.128399</v>
-      </c>
-      <c r="H66" t="s">
-        <v>14</v>
-      </c>
       <c r="I66">
         <v>30000</v>
       </c>
@@ -2600,59 +2632,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="B67">
-        <v>23489.058471749791</v>
+        <v>22536.048287109341</v>
       </c>
       <c r="C67">
         <v>0.5</v>
       </c>
       <c r="D67">
-        <v>25325388674.277729</v>
+        <v>19661964823.227219</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F67">
         <v>2000</v>
       </c>
       <c r="G67">
-        <v>22144092284.99855</v>
+        <v>-8479448721.7418594</v>
       </c>
       <c r="H67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I67">
         <v>30000</v>
       </c>
       <c r="J67">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="B68">
-        <v>26116.61664329467</v>
+        <v>84501.197139652882</v>
       </c>
       <c r="C68">
         <v>0.5</v>
       </c>
       <c r="D68">
-        <v>25476088775.11676</v>
+        <v>45611555088.877579</v>
       </c>
       <c r="E68" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F68">
         <v>2000</v>
       </c>
       <c r="G68">
-        <v>22077699853.435921</v>
+        <v>36444544761.734222</v>
       </c>
       <c r="H68" t="s">
         <v>19</v>
@@ -2664,36 +2696,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="B69">
-        <v>27065.314384988142</v>
+        <v>23125.87847440011</v>
       </c>
       <c r="C69">
         <v>0.5</v>
       </c>
       <c r="D69">
-        <v>25324156658.592831</v>
+        <v>19288153411.084431</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F69">
         <v>2000</v>
       </c>
       <c r="G69">
-        <v>21991799433.5061</v>
+        <v>-9546945430.0797501</v>
       </c>
       <c r="H69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I69">
         <v>30000</v>
       </c>
       <c r="J69">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -3016,62 +3048,62 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="B80">
-        <v>26116.61664329467</v>
+        <v>77635.159985174396</v>
       </c>
       <c r="C80">
         <v>0.5</v>
       </c>
       <c r="D80">
-        <v>25476088775.11676</v>
+        <v>45552330647.758202</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F80">
         <v>2000</v>
       </c>
       <c r="G80">
-        <v>-7067684326.9366112</v>
+        <v>36143251421.835648</v>
       </c>
       <c r="H80" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I80">
         <v>30000</v>
       </c>
       <c r="J80">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="B81">
-        <v>22108.275274640881</v>
+        <v>23352.711087550659</v>
       </c>
       <c r="C81">
         <v>0.5</v>
       </c>
       <c r="D81">
-        <v>20035862225.05909</v>
+        <v>11411382815.65556</v>
       </c>
       <c r="E81" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F81">
         <v>2000</v>
       </c>
       <c r="G81">
-        <v>-7731752722.8577595</v>
+        <v>-17540882769.420479</v>
       </c>
       <c r="H81" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I81">
         <v>30000</v>
@@ -3080,62 +3112,62 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="B82">
-        <v>27065.314384988142</v>
+        <v>77972.636944767553</v>
       </c>
       <c r="C82">
         <v>0.5</v>
       </c>
       <c r="D82">
-        <v>25324156658.592831</v>
+        <v>45517080550.665993</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F82">
         <v>2000</v>
       </c>
       <c r="G82">
-        <v>-8212303819.4920578</v>
+        <v>36060638338.974571</v>
       </c>
       <c r="H82" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I82">
         <v>30000</v>
       </c>
       <c r="J82">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B83">
-        <v>22536.048287109341</v>
+        <v>23411.004095767919</v>
       </c>
       <c r="C83">
         <v>0.5</v>
       </c>
       <c r="D83">
-        <v>19661964823.227219</v>
+        <v>25382547065.410648</v>
       </c>
       <c r="E83" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F83">
         <v>2000</v>
       </c>
       <c r="G83">
-        <v>-8479448721.7418594</v>
+        <v>-3918792411.5294151</v>
       </c>
       <c r="H83" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I83">
         <v>30000</v>
@@ -3144,62 +3176,60 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="B84">
-        <v>23125.87847440011</v>
+        <v>80292.148994584961</v>
       </c>
       <c r="C84">
         <v>0.5</v>
       </c>
       <c r="D84">
-        <v>19288153411.084431</v>
+        <v>45500943700.806664</v>
       </c>
       <c r="E84" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F84">
         <v>2000</v>
       </c>
       <c r="G84">
-        <v>-9546945430.0797501</v>
+        <v>35945493931.87793</v>
       </c>
       <c r="H84" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I84">
         <v>30000</v>
       </c>
       <c r="J84">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A85" s="1">
-        <v>78</v>
-      </c>
+      <c r="A85" s="2"/>
       <c r="B85">
-        <v>23968.6981179799</v>
+        <v>23440.341222798532</v>
       </c>
       <c r="C85">
         <v>0.5</v>
       </c>
       <c r="D85">
-        <v>19022322726.398029</v>
+        <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F85">
         <v>2000</v>
       </c>
-      <c r="G85">
-        <v>-10698818206.98875</v>
+      <c r="G85" s="4">
+        <v>-29006713587.66103</v>
       </c>
       <c r="H85" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I85">
         <v>30000</v>
@@ -3208,18 +3238,18 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B86">
-        <v>30023.950497196631</v>
+        <v>24063.7167217729</v>
       </c>
       <c r="C86">
         <v>0.5</v>
       </c>
       <c r="D86">
-        <v>25323638096.75692</v>
+        <v>26038427122.019909</v>
       </c>
       <c r="E86" t="s">
         <v>11</v>
@@ -3228,106 +3258,104 @@
         <v>2000</v>
       </c>
       <c r="G86">
-        <v>-11587106010.587521</v>
+        <v>22599840289.700722</v>
       </c>
       <c r="H86" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I86">
         <v>30000</v>
       </c>
       <c r="J86">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="B87">
-        <v>20626.669741520309</v>
+        <v>23489.058471749791</v>
       </c>
       <c r="C87">
         <v>0.5</v>
       </c>
       <c r="D87">
-        <v>12793685173.17964</v>
+        <v>25325388674.277729</v>
       </c>
       <c r="E87" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F87">
         <v>2000</v>
       </c>
       <c r="G87">
-        <v>-13189800236.28256</v>
+        <v>-4069013437.8726912</v>
       </c>
       <c r="H87" t="s">
+        <v>13</v>
+      </c>
+      <c r="I87">
+        <v>30000</v>
+      </c>
+      <c r="J87">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>14</v>
+      </c>
+      <c r="B88">
+        <v>23903.872474536049</v>
+      </c>
+      <c r="C88">
+        <v>0.5</v>
+      </c>
+      <c r="D88">
+        <v>25943991993.935848</v>
+      </c>
+      <c r="E88" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88">
+        <v>2000</v>
+      </c>
+      <c r="G88">
+        <v>22517654927.29821</v>
+      </c>
+      <c r="H88" t="s">
         <v>16</v>
       </c>
-      <c r="I87">
-        <v>30000</v>
-      </c>
-      <c r="J87">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A88" s="1">
-        <v>115</v>
-      </c>
-      <c r="B88">
-        <v>20822.087903888802</v>
-      </c>
-      <c r="C88">
-        <v>0.5</v>
-      </c>
-      <c r="D88">
-        <v>13004979207.748819</v>
-      </c>
-      <c r="E88" t="s">
-        <v>23</v>
-      </c>
-      <c r="F88">
-        <v>2000</v>
-      </c>
-      <c r="G88">
-        <v>-13212072478.742279</v>
-      </c>
-      <c r="H88" t="s">
-        <v>17</v>
-      </c>
       <c r="I88">
         <v>30000</v>
       </c>
       <c r="J88">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" s="1">
-        <v>79</v>
-      </c>
+      <c r="A89" s="2"/>
       <c r="B89">
-        <v>26529.914723114511</v>
+        <v>23724.104954962881</v>
       </c>
       <c r="C89">
         <v>0.5</v>
       </c>
       <c r="D89">
-        <v>19021961642.033379</v>
+        <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="F89">
         <v>2000</v>
       </c>
-      <c r="G89">
-        <v>-13615321452.680321</v>
+      <c r="G89" s="4">
+        <v>-29863687044.677849</v>
       </c>
       <c r="H89" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="I89">
         <v>30000</v>
@@ -3658,16 +3686,16 @@
     </row>
     <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B100">
-        <v>30023.950497196631</v>
+        <v>24982.28481735395</v>
       </c>
       <c r="C100">
         <v>0.5</v>
       </c>
       <c r="D100">
-        <v>25323638096.75692</v>
+        <v>25907854092.22858</v>
       </c>
       <c r="E100" t="s">
         <v>11</v>
@@ -3676,10 +3704,10 @@
         <v>2000</v>
       </c>
       <c r="G100">
-        <v>21918749047.324459</v>
+        <v>22428154763.56657</v>
       </c>
       <c r="H100" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I100">
         <v>30000</v>
@@ -3688,123 +3716,123 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="B101">
-        <v>21361.217460565149</v>
+        <v>23769.053028574359</v>
       </c>
       <c r="C101">
         <v>0.5</v>
       </c>
       <c r="D101">
-        <v>20267332536.053719</v>
+        <v>25603298136.0681</v>
       </c>
       <c r="E101" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F101">
         <v>2000</v>
       </c>
       <c r="G101">
-        <v>17202926625.051601</v>
+        <v>-4199008720.5531378</v>
       </c>
       <c r="H101" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I101">
         <v>30000</v>
       </c>
       <c r="J101">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="B102">
-        <v>21171.225055369079</v>
+        <v>23769.053028574359</v>
       </c>
       <c r="C102">
         <v>0.5</v>
       </c>
       <c r="D102">
-        <v>20101614053.26363</v>
+        <v>25603298136.0681</v>
       </c>
       <c r="E102" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F102">
         <v>2000</v>
       </c>
       <c r="G102">
-        <v>17052464163.29565</v>
+        <v>22326562779.892719</v>
       </c>
       <c r="H102" t="s">
+        <v>15</v>
+      </c>
+      <c r="I102">
+        <v>30000</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>34</v>
+      </c>
+      <c r="B103">
+        <v>23903.872474536049</v>
+      </c>
+      <c r="C103">
+        <v>0.5</v>
+      </c>
+      <c r="D103">
+        <v>25943991993.935848</v>
+      </c>
+      <c r="E103" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103">
+        <v>2000</v>
+      </c>
+      <c r="G103">
+        <v>-4158371151.5950012</v>
+      </c>
+      <c r="H103" t="s">
         <v>16</v>
       </c>
-      <c r="I102">
-        <v>30000</v>
-      </c>
-      <c r="J102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="1">
-        <v>56</v>
-      </c>
-      <c r="B103">
-        <v>22108.275274640881</v>
-      </c>
-      <c r="C103">
-        <v>0.5</v>
-      </c>
-      <c r="D103">
-        <v>20035862225.05909</v>
-      </c>
-      <c r="E103" t="s">
-        <v>22</v>
-      </c>
-      <c r="F103">
-        <v>2000</v>
-      </c>
-      <c r="G103">
-        <v>16940439132.83099</v>
-      </c>
-      <c r="H103" t="s">
-        <v>18</v>
-      </c>
       <c r="I103">
         <v>30000</v>
       </c>
       <c r="J103">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="B104">
-        <v>22536.048287109341</v>
+        <v>25443.990488585241</v>
       </c>
       <c r="C104">
         <v>0.5</v>
       </c>
       <c r="D104">
-        <v>19661964823.227219</v>
+        <v>25681265238.053619</v>
       </c>
       <c r="E104" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F104">
         <v>2000</v>
       </c>
       <c r="G104">
-        <v>16670125367.667021</v>
+        <v>22322413506.488419</v>
       </c>
       <c r="H104" t="s">
         <v>12</v>
@@ -3816,18 +3844,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="B105">
-        <v>21005.698396268748</v>
+        <v>23968.6981179799</v>
       </c>
       <c r="C105">
         <v>0.5</v>
       </c>
       <c r="D105">
-        <v>19498702822.720089</v>
+        <v>19022322726.398029</v>
       </c>
       <c r="E105" t="s">
         <v>22</v>
@@ -3836,39 +3864,39 @@
         <v>2000</v>
       </c>
       <c r="G105">
-        <v>16586731835.19878</v>
+        <v>-10698818206.98875</v>
       </c>
       <c r="H105" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I105">
         <v>30000</v>
       </c>
       <c r="J105">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="B106">
-        <v>20684.83304849601</v>
+        <v>23411.004095767919</v>
       </c>
       <c r="C106">
         <v>0.5</v>
       </c>
       <c r="D106">
-        <v>19121303093.281639</v>
+        <v>25382547065.410648</v>
       </c>
       <c r="E106" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F106">
         <v>2000</v>
       </c>
       <c r="G106">
-        <v>16300471876.809629</v>
+        <v>22207206899.128399</v>
       </c>
       <c r="H106" t="s">
         <v>14</v>
@@ -3880,59 +3908,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B107">
-        <v>23125.87847440011</v>
+        <v>24063.7167217729</v>
       </c>
       <c r="C107">
         <v>0.5</v>
       </c>
       <c r="D107">
-        <v>19288153411.084431</v>
+        <v>26038427122.019909</v>
       </c>
       <c r="E107" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F107">
         <v>2000</v>
       </c>
       <c r="G107">
-        <v>16260861984.28718</v>
+        <v>-4254567317.6411929</v>
       </c>
       <c r="H107" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I107">
         <v>30000</v>
       </c>
       <c r="J107">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B108">
-        <v>20750.62089947232</v>
+        <v>23489.058471749791</v>
       </c>
       <c r="C108">
         <v>0.5</v>
       </c>
       <c r="D108">
-        <v>19023392633.209332</v>
+        <v>25325388674.277729</v>
       </c>
       <c r="E108" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F108">
         <v>2000</v>
       </c>
       <c r="G108">
-        <v>16197422609.60181</v>
+        <v>22144092284.99855</v>
       </c>
       <c r="H108" t="s">
         <v>13</v>
@@ -3944,36 +3972,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="1">
-        <v>58</v>
-      </c>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="2"/>
       <c r="B109">
-        <v>23968.6981179799</v>
+        <v>24066.91794378401</v>
       </c>
       <c r="C109">
         <v>0.5</v>
       </c>
       <c r="D109">
-        <v>19022322726.398029</v>
+        <v>0</v>
       </c>
       <c r="E109" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F109">
         <v>2000</v>
       </c>
-      <c r="G109">
-        <v>16049551403.56159</v>
+      <c r="G109" s="4">
+        <v>-29762704211.95647</v>
       </c>
       <c r="H109" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I109">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="J109">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4296,123 +4322,121 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="B120">
-        <v>20464.017846168768</v>
+        <v>26116.61664329467</v>
       </c>
       <c r="C120">
         <v>0.5</v>
       </c>
       <c r="D120">
-        <v>12020589552.05784</v>
+        <v>25476088775.11676</v>
       </c>
       <c r="E120" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F120">
         <v>2000</v>
       </c>
       <c r="G120">
-        <v>-13648043017.20833</v>
+        <v>22077699853.435921</v>
       </c>
       <c r="H120" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I120">
         <v>30000</v>
       </c>
       <c r="J120">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A121" s="1">
-        <v>112</v>
-      </c>
+      <c r="A121" s="2"/>
       <c r="B121">
-        <v>20141.275508210809</v>
+        <v>24357.233708533258</v>
       </c>
       <c r="C121">
         <v>0.5</v>
       </c>
       <c r="D121">
-        <v>11538656672.076599</v>
+        <v>0</v>
       </c>
       <c r="E121" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="F121">
         <v>2000</v>
       </c>
-      <c r="G121">
-        <v>-13679618070.55022</v>
+      <c r="G121" s="4">
+        <v>-30640596520.949848</v>
       </c>
       <c r="H121" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I121">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="J121">
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="B122">
-        <v>20204.21675520407</v>
+        <v>27065.314384988142</v>
       </c>
       <c r="C122">
         <v>0.5</v>
       </c>
       <c r="D122">
-        <v>11412353729.80073</v>
+        <v>25324156658.592831</v>
       </c>
       <c r="E122" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F122">
         <v>2000</v>
       </c>
       <c r="G122">
-        <v>-13881106520.16177</v>
+        <v>21991799433.5061</v>
       </c>
       <c r="H122" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I122">
         <v>30000</v>
       </c>
       <c r="J122">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>116</v>
+        <v>36</v>
       </c>
       <c r="B123">
-        <v>21534.299247355699</v>
+        <v>24982.28481735395</v>
       </c>
       <c r="C123">
         <v>0.5</v>
       </c>
       <c r="D123">
-        <v>12710451017.524389</v>
+        <v>25907854092.22858</v>
       </c>
       <c r="E123" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F123">
         <v>2000</v>
       </c>
       <c r="G123">
-        <v>-14330625586.991381</v>
+        <v>-5451348108.1122684</v>
       </c>
       <c r="H123" t="s">
         <v>18</v>
@@ -4424,62 +4448,62 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="B124">
-        <v>21949.020584726932</v>
+        <v>30023.950497196631</v>
       </c>
       <c r="C124">
         <v>0.5</v>
       </c>
       <c r="D124">
-        <v>12230213709.06971</v>
+        <v>25323638096.75692</v>
       </c>
       <c r="E124" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F124">
         <v>2000</v>
       </c>
       <c r="G124">
-        <v>-15173292308.438351</v>
+        <v>21918749047.324459</v>
       </c>
       <c r="H124" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="I124">
         <v>30000</v>
       </c>
       <c r="J124">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="B125">
-        <v>22530.550530083208</v>
+        <v>25443.990488585241</v>
       </c>
       <c r="C125">
         <v>0.5</v>
       </c>
       <c r="D125">
-        <v>11755267387.44474</v>
+        <v>25681265238.053619</v>
       </c>
       <c r="E125" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F125">
         <v>2000</v>
       </c>
       <c r="G125">
-        <v>-16332423617.94474</v>
+        <v>-6072339458.6494951</v>
       </c>
       <c r="H125" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I125">
         <v>30000</v>
@@ -4488,62 +4512,62 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>118</v>
+        <v>55</v>
       </c>
       <c r="B126">
-        <v>23352.711087550659</v>
+        <v>21361.217460565149</v>
       </c>
       <c r="C126">
         <v>0.5</v>
       </c>
       <c r="D126">
-        <v>11411382815.65556</v>
+        <v>20267332536.053719</v>
       </c>
       <c r="E126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F126">
         <v>2000</v>
       </c>
       <c r="G126">
-        <v>-17540882769.420479</v>
+        <v>17202926625.051601</v>
       </c>
       <c r="H126" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I126">
         <v>30000</v>
       </c>
       <c r="J126">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="B127">
-        <v>46775.887056236512</v>
+        <v>25790.727244949579</v>
       </c>
       <c r="C127">
         <v>0.5</v>
       </c>
       <c r="D127">
-        <v>38496156221.228981</v>
+        <v>11411109391.88575</v>
       </c>
       <c r="E127" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F127">
         <v>2000</v>
       </c>
       <c r="G127">
-        <v>-19275777046.16238</v>
+        <v>-20316611094.87289</v>
       </c>
       <c r="H127" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="I127">
         <v>30000</v>
@@ -4554,28 +4578,28 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>119</v>
+        <v>37</v>
       </c>
       <c r="B128">
-        <v>25790.727244949579</v>
+        <v>26116.61664329467</v>
       </c>
       <c r="C128">
         <v>0.5</v>
       </c>
       <c r="D128">
-        <v>11411109391.88575</v>
+        <v>25476088775.11676</v>
       </c>
       <c r="E128" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F128">
         <v>2000</v>
       </c>
       <c r="G128">
-        <v>-20316611094.87289</v>
+        <v>-7067684326.9366112</v>
       </c>
       <c r="H128" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I128">
         <v>30000</v>
@@ -4586,28 +4610,28 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="B129">
-        <v>47238.628680518457</v>
+        <v>26529.914723114511</v>
       </c>
       <c r="C129">
         <v>0.5</v>
       </c>
       <c r="D129">
-        <v>38487562808.205406</v>
+        <v>19021961642.033379</v>
       </c>
       <c r="E129" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F129">
         <v>2000</v>
       </c>
       <c r="G129">
-        <v>-20801248369.261429</v>
+        <v>-13615321452.680321</v>
       </c>
       <c r="H129" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="I129">
         <v>30000</v>
@@ -4936,190 +4960,184 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B140">
-        <v>26529.914723114511</v>
+        <v>27065.314384988142</v>
       </c>
       <c r="C140">
         <v>0.5</v>
       </c>
       <c r="D140">
-        <v>19021961642.033379</v>
+        <v>25324156658.592831</v>
       </c>
       <c r="E140" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F140">
         <v>2000</v>
       </c>
       <c r="G140">
-        <v>15991291357.797029</v>
+        <v>-8212303819.4920578</v>
       </c>
       <c r="H140" t="s">
+        <v>20</v>
+      </c>
+      <c r="I140">
+        <v>30000</v>
+      </c>
+      <c r="J140">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>39</v>
+      </c>
+      <c r="B141">
+        <v>30023.950497196631</v>
+      </c>
+      <c r="C141">
+        <v>0.5</v>
+      </c>
+      <c r="D141">
+        <v>25323638096.75692</v>
+      </c>
+      <c r="E141" t="s">
+        <v>11</v>
+      </c>
+      <c r="F141">
+        <v>2000</v>
+      </c>
+      <c r="G141">
+        <v>-11587106010.587521</v>
+      </c>
+      <c r="H141" t="s">
         <v>21</v>
       </c>
-      <c r="I140">
-        <v>30000</v>
-      </c>
-      <c r="J140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="1">
-        <v>95</v>
-      </c>
-      <c r="B141">
-        <v>20822.087903888802</v>
-      </c>
-      <c r="C141">
-        <v>0.5</v>
-      </c>
-      <c r="D141">
-        <v>13004979207.748819</v>
-      </c>
-      <c r="E141" t="s">
-        <v>23</v>
-      </c>
-      <c r="F141">
-        <v>2000</v>
-      </c>
-      <c r="G141">
-        <v>10024771699.23962</v>
-      </c>
-      <c r="H141" t="s">
-        <v>17</v>
-      </c>
       <c r="I141">
         <v>30000</v>
       </c>
       <c r="J141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="1">
-        <v>94</v>
-      </c>
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A142" s="2"/>
       <c r="B142">
-        <v>20626.669741520309</v>
+        <v>41638.412618282797</v>
       </c>
       <c r="C142">
         <v>0.5</v>
       </c>
       <c r="D142">
-        <v>12793685173.17964</v>
+        <v>43958817798.719643</v>
       </c>
       <c r="E142" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F142">
         <v>2000</v>
       </c>
       <c r="G142">
-        <v>9828962959.1646347</v>
+        <v>-7988875075.8882494</v>
       </c>
       <c r="H142" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I142">
         <v>30000</v>
       </c>
       <c r="J142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="1">
-        <v>96</v>
-      </c>
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A143" s="2"/>
       <c r="B143">
-        <v>21534.299247355699</v>
+        <v>42052.161729027488</v>
       </c>
       <c r="C143">
         <v>0.5</v>
       </c>
       <c r="D143">
-        <v>12710451017.524389</v>
+        <v>43950888085.400322</v>
       </c>
       <c r="E143" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F143">
         <v>2000</v>
       </c>
       <c r="G143">
-        <v>9701025724.949482</v>
+        <v>-9370885211.4656467</v>
       </c>
       <c r="H143" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I143">
         <v>30000</v>
       </c>
       <c r="J143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="1">
-        <v>90</v>
-      </c>
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A144" s="2"/>
       <c r="B144">
-        <v>21949.020584726932</v>
+        <v>42858.988719474743</v>
       </c>
       <c r="C144">
         <v>0.5</v>
       </c>
       <c r="D144">
-        <v>12230213709.06971</v>
+        <v>44481746991.048927</v>
       </c>
       <c r="E144" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F144">
         <v>2000</v>
       </c>
       <c r="G144">
-        <v>9321175947.6178722</v>
+        <v>-9005270461.8120232</v>
       </c>
       <c r="H144" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I144">
         <v>30000</v>
       </c>
       <c r="J144">
-        <v>0</v>
+        <v>1115970.8999999999</v>
       </c>
     </row>
     <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="B145">
-        <v>20464.017846168768</v>
+        <v>21171.225055369079</v>
       </c>
       <c r="C145">
         <v>0.5</v>
       </c>
       <c r="D145">
-        <v>12020589552.05784</v>
+        <v>20101614053.26363</v>
       </c>
       <c r="E145" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F145">
         <v>2000</v>
       </c>
       <c r="G145">
-        <v>9189205396.1966839</v>
+        <v>17052464163.29565</v>
       </c>
       <c r="H145" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I145">
         <v>30000</v>
@@ -5130,28 +5148,28 @@
     </row>
     <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="B146">
-        <v>22530.550530083208</v>
+        <v>22108.275274640881</v>
       </c>
       <c r="C146">
         <v>0.5</v>
       </c>
       <c r="D146">
-        <v>11755267387.44474</v>
+        <v>20035862225.05909</v>
       </c>
       <c r="E146" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F146">
         <v>2000</v>
       </c>
       <c r="G146">
-        <v>8811015134.6077042</v>
+        <v>16940439132.83099</v>
       </c>
       <c r="H146" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I146">
         <v>30000</v>
@@ -5162,28 +5180,28 @@
     </row>
     <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="B147">
-        <v>20141.275508210809</v>
+        <v>22536.048287109341</v>
       </c>
       <c r="C147">
         <v>0.5</v>
       </c>
       <c r="D147">
-        <v>11538656672.076599</v>
+        <v>19661964823.227219</v>
       </c>
       <c r="E147" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F147">
         <v>2000</v>
       </c>
       <c r="G147">
-        <v>8797459285.4957466</v>
+        <v>16670125367.667021</v>
       </c>
       <c r="H147" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I147">
         <v>30000</v>
@@ -5194,28 +5212,28 @@
     </row>
     <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="B148">
-        <v>20204.21675520407</v>
+        <v>21005.698396268748</v>
       </c>
       <c r="C148">
         <v>0.5</v>
       </c>
       <c r="D148">
-        <v>11412353729.80073</v>
+        <v>19498702822.720089</v>
       </c>
       <c r="E148" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F148">
         <v>2000</v>
       </c>
       <c r="G148">
-        <v>8666211435.9383888</v>
+        <v>16586731835.19878</v>
       </c>
       <c r="H148" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I148">
         <v>30000</v>
@@ -5226,28 +5244,28 @@
     </row>
     <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="B149">
-        <v>23352.711087550659</v>
+        <v>20684.83304849601</v>
       </c>
       <c r="C149">
         <v>0.5</v>
       </c>
       <c r="D149">
-        <v>11411382815.65556</v>
+        <v>19121303093.281639</v>
       </c>
       <c r="E149" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F149">
         <v>2000</v>
       </c>
       <c r="G149">
-        <v>8520063240.3933992</v>
+        <v>16300471876.809629</v>
       </c>
       <c r="H149" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I149">
         <v>30000</v>
@@ -5576,57 +5594,59 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A160" s="2"/>
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>57</v>
+      </c>
       <c r="B160">
-        <v>59987.272186896596</v>
+        <v>23125.87847440011</v>
       </c>
       <c r="C160">
         <v>0.5</v>
       </c>
       <c r="D160">
-        <v>40245166908.101097</v>
+        <v>19288153411.084431</v>
       </c>
       <c r="E160" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F160">
         <v>2000</v>
       </c>
       <c r="G160">
-        <v>-33120050883.821098</v>
+        <v>16260861984.28718</v>
       </c>
       <c r="H160" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I160">
         <v>30000</v>
       </c>
       <c r="J160">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>151</v>
+        <v>51</v>
       </c>
       <c r="B161">
-        <v>76493.02222308013</v>
+        <v>20750.62089947232</v>
       </c>
       <c r="C161">
         <v>0.5</v>
       </c>
       <c r="D161">
-        <v>45692670299.384941</v>
+        <v>19023392633.209332</v>
       </c>
       <c r="E161" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F161">
         <v>2000</v>
       </c>
       <c r="G161">
-        <v>-48427670965.711304</v>
+        <v>16197422609.60181</v>
       </c>
       <c r="H161" t="s">
         <v>13</v>
@@ -5635,65 +5655,63 @@
         <v>30000</v>
       </c>
       <c r="J161">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="B162">
-        <v>76468.966708554668</v>
+        <v>23968.6981179799</v>
       </c>
       <c r="C162">
         <v>0.5</v>
       </c>
       <c r="D162">
-        <v>45681872443.045227</v>
+        <v>19022322726.398029</v>
       </c>
       <c r="E162" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F162">
         <v>2000</v>
       </c>
       <c r="G162">
-        <v>-48436496182.323822</v>
+        <v>16049551403.56159</v>
       </c>
       <c r="H162" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I162">
         <v>30000</v>
       </c>
       <c r="J162">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A163" s="1">
-        <v>153</v>
-      </c>
+      <c r="A163" s="2"/>
       <c r="B163">
-        <v>76853.387521036348</v>
+        <v>43271.663230891158</v>
       </c>
       <c r="C163">
         <v>0.5</v>
       </c>
       <c r="D163">
-        <v>45630534694.182037</v>
+        <v>44474089301.108017</v>
       </c>
       <c r="E163" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F163">
         <v>2000</v>
       </c>
       <c r="G163">
-        <v>-49126963663.181602</v>
+        <v>-10412992137.455759</v>
       </c>
       <c r="H163" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I163">
         <v>30000</v>
@@ -5702,97 +5720,93 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A164" s="1">
-        <v>154</v>
-      </c>
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="2"/>
       <c r="B164">
-        <v>77635.159985174396</v>
+        <v>53903.196729560907</v>
       </c>
       <c r="C164">
         <v>0.5</v>
       </c>
       <c r="D164">
-        <v>45552330647.758202</v>
+        <v>36152247074.781609</v>
       </c>
       <c r="E164" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F164">
         <v>2000</v>
       </c>
       <c r="G164">
-        <v>-50495327938.463402</v>
+        <v>-29941568211.32774</v>
       </c>
       <c r="H164" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I164">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="J164">
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="B165">
-        <v>77972.636944767553</v>
+        <v>26529.914723114511</v>
       </c>
       <c r="C165">
         <v>0.5</v>
       </c>
       <c r="D165">
-        <v>45517080550.665993</v>
+        <v>19021961642.033379</v>
       </c>
       <c r="E165" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F165">
         <v>2000</v>
       </c>
       <c r="G165">
-        <v>-50954555487.650848</v>
+        <v>15991291357.797029</v>
       </c>
       <c r="H165" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I165">
         <v>30000</v>
       </c>
       <c r="J165">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A166" s="1">
-        <v>156</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="2"/>
       <c r="B166">
-        <v>80292.148994584961</v>
+        <v>54410.325563740516</v>
       </c>
       <c r="C166">
         <v>0.5</v>
       </c>
       <c r="D166">
-        <v>45500943700.806664</v>
+        <v>36142898870.665154</v>
       </c>
       <c r="E166" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F166">
         <v>2000</v>
       </c>
       <c r="G166">
-        <v>-53658207844.543114</v>
+        <v>-31624764918.147991</v>
       </c>
       <c r="H166" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I166">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="J166">
         <v>1115970.8999999999</v>
@@ -5800,28 +5814,28 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>150</v>
+        <v>6</v>
       </c>
       <c r="B167">
-        <v>82759.777568824735</v>
+        <v>46775.887056236512</v>
       </c>
       <c r="C167">
         <v>0.5</v>
       </c>
       <c r="D167">
-        <v>45624202826.455658</v>
+        <v>38496156221.228981</v>
       </c>
       <c r="E167" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F167">
         <v>2000</v>
       </c>
       <c r="G167">
-        <v>-55809608702.400337</v>
+        <v>-19275777046.16238</v>
       </c>
       <c r="H167" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I167">
         <v>30000</v>
@@ -5830,62 +5844,62 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>157</v>
+        <v>95</v>
       </c>
       <c r="B168">
-        <v>84501.197139652882</v>
+        <v>20822.087903888802</v>
       </c>
       <c r="C168">
         <v>0.5</v>
       </c>
       <c r="D168">
-        <v>45611555088.877579</v>
+        <v>13004979207.748819</v>
       </c>
       <c r="E168" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F168">
         <v>2000</v>
       </c>
       <c r="G168">
-        <v>-57856332261.281601</v>
+        <v>10024771699.23962</v>
       </c>
       <c r="H168" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I168">
         <v>30000</v>
       </c>
       <c r="J168">
-        <v>1115970.8999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>158</v>
+        <v>7</v>
       </c>
       <c r="B169">
-        <v>89519.889499620855</v>
+        <v>47238.628680518457</v>
       </c>
       <c r="C169">
         <v>0.5</v>
       </c>
       <c r="D169">
-        <v>45692079294.099579</v>
+        <v>38487562808.205406</v>
       </c>
       <c r="E169" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F169">
         <v>2000</v>
       </c>
       <c r="G169">
-        <v>-63012463750.982613</v>
+        <v>-20801248369.261429</v>
       </c>
       <c r="H169" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I169">
         <v>30000</v>
@@ -5894,108 +5908,110 @@
         <v>1115970.8999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="B170">
-        <v>104513.00660286591</v>
+        <v>20626.669741520309</v>
       </c>
       <c r="C170">
         <v>0.5</v>
       </c>
       <c r="D170">
-        <v>45691116442.457909</v>
+        <v>12793685173.17964</v>
       </c>
       <c r="E170" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F170">
         <v>2000</v>
       </c>
       <c r="G170">
-        <v>-79806248476.391983</v>
+        <v>9828962959.1646347</v>
       </c>
       <c r="H170" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I170">
         <v>30000</v>
       </c>
       <c r="J170">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="1">
-        <v>99</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A171" s="2"/>
       <c r="B171">
-        <v>25790.727244949579</v>
+        <v>52316.086802824248</v>
       </c>
       <c r="C171">
         <v>0.5</v>
       </c>
       <c r="D171">
-        <v>11411109391.88575</v>
+        <v>33833532056.768509</v>
       </c>
       <c r="E171" t="s">
+        <v>27</v>
+      </c>
+      <c r="F171">
+        <v>2000</v>
+      </c>
+      <c r="G171">
+        <v>-30318561389.1497</v>
+      </c>
+      <c r="H171" t="s">
+        <v>9</v>
+      </c>
+      <c r="I171">
+        <v>30000</v>
+      </c>
+      <c r="J171">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="3">
+        <v>96</v>
+      </c>
+      <c r="B172">
+        <v>21534.299247355699</v>
+      </c>
+      <c r="C172">
+        <v>0.5</v>
+      </c>
+      <c r="D172">
+        <v>12710451017.524389</v>
+      </c>
+      <c r="E172" t="s">
         <v>23</v>
       </c>
-      <c r="F171">
-        <v>2000</v>
-      </c>
-      <c r="G171">
-        <v>8465090000.3280087</v>
-      </c>
-      <c r="H171" t="s">
-        <v>21</v>
-      </c>
-      <c r="I171">
-        <v>30000</v>
-      </c>
-      <c r="J171">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B172">
-        <v>59907.386841751548</v>
-      </c>
-      <c r="C172">
-        <v>0.5</v>
-      </c>
-      <c r="D172">
-        <v>45669430836.814667</v>
-      </c>
-      <c r="E172" t="s">
-        <v>27</v>
-      </c>
       <c r="F172">
         <v>2000</v>
       </c>
       <c r="G172">
-        <v>39345493500.230591</v>
+        <v>9701025724.949482</v>
       </c>
       <c r="H172" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I172">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="J172">
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A173" s="5"/>
       <c r="B173">
-        <v>60452.209425135603</v>
+        <v>52818.955692821633</v>
       </c>
       <c r="C173">
         <v>0.5</v>
       </c>
       <c r="D173">
-        <v>45661151303.619812</v>
+        <v>33824347003.661751</v>
       </c>
       <c r="E173" t="s">
         <v>28</v>
@@ -6004,194 +6020,942 @@
         <v>2000</v>
       </c>
       <c r="G173">
-        <v>37804064360.125252</v>
+        <v>-31979931245.781521</v>
       </c>
       <c r="H173" t="s">
         <v>9</v>
       </c>
       <c r="I173">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="J173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="3">
+        <v>90</v>
+      </c>
       <c r="B174">
-        <v>67445.186139135913</v>
+        <v>21949.020584726932</v>
       </c>
       <c r="C174">
         <v>0.5</v>
       </c>
       <c r="D174">
-        <v>45634079074.988136</v>
+        <v>12230213709.06971</v>
       </c>
       <c r="E174" t="s">
+        <v>23</v>
+      </c>
+      <c r="F174">
+        <v>2000</v>
+      </c>
+      <c r="G174">
+        <v>9321175947.6178722</v>
+      </c>
+      <c r="H174" t="s">
+        <v>12</v>
+      </c>
+      <c r="I174">
+        <v>30000</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A175" s="5"/>
+      <c r="B175">
+        <v>59987.272186896596</v>
+      </c>
+      <c r="C175">
+        <v>0.5</v>
+      </c>
+      <c r="D175">
+        <v>40245166908.101097</v>
+      </c>
+      <c r="E175" t="s">
+        <v>25</v>
+      </c>
+      <c r="F175">
+        <v>2000</v>
+      </c>
+      <c r="G175">
+        <v>-33120050883.821098</v>
+      </c>
+      <c r="H175" t="s">
+        <v>26</v>
+      </c>
+      <c r="I175">
+        <v>30000</v>
+      </c>
+      <c r="J175">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="3">
+        <v>93</v>
+      </c>
+      <c r="B176">
+        <v>20464.017846168768</v>
+      </c>
+      <c r="C176">
+        <v>0.5</v>
+      </c>
+      <c r="D176">
+        <v>12020589552.05784</v>
+      </c>
+      <c r="E176" t="s">
+        <v>23</v>
+      </c>
+      <c r="F176">
+        <v>2000</v>
+      </c>
+      <c r="G176">
+        <v>9189205396.1966839</v>
+      </c>
+      <c r="H176" t="s">
+        <v>15</v>
+      </c>
+      <c r="I176">
+        <v>30000</v>
+      </c>
+      <c r="J176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A177" s="3">
+        <v>152</v>
+      </c>
+      <c r="B177">
+        <v>76468.966708554668</v>
+      </c>
+      <c r="C177">
+        <v>0.5</v>
+      </c>
+      <c r="D177">
+        <v>45681872443.045227</v>
+      </c>
+      <c r="E177" t="s">
+        <v>24</v>
+      </c>
+      <c r="F177">
+        <v>2000</v>
+      </c>
+      <c r="G177">
+        <v>-48436496182.323822</v>
+      </c>
+      <c r="H177" t="s">
+        <v>14</v>
+      </c>
+      <c r="I177">
+        <v>30000</v>
+      </c>
+      <c r="J177">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="3">
+        <v>97</v>
+      </c>
+      <c r="B178">
+        <v>22530.550530083208</v>
+      </c>
+      <c r="C178">
+        <v>0.5</v>
+      </c>
+      <c r="D178">
+        <v>11755267387.44474</v>
+      </c>
+      <c r="E178" t="s">
+        <v>23</v>
+      </c>
+      <c r="F178">
+        <v>2000</v>
+      </c>
+      <c r="G178">
+        <v>8811015134.6077042</v>
+      </c>
+      <c r="H178" t="s">
+        <v>19</v>
+      </c>
+      <c r="I178">
+        <v>30000</v>
+      </c>
+      <c r="J178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A179" s="3">
+        <v>151</v>
+      </c>
+      <c r="B179">
+        <v>76493.02222308013</v>
+      </c>
+      <c r="C179">
+        <v>0.5</v>
+      </c>
+      <c r="D179">
+        <v>45692670299.384941</v>
+      </c>
+      <c r="E179" t="s">
+        <v>24</v>
+      </c>
+      <c r="F179">
+        <v>2000</v>
+      </c>
+      <c r="G179">
+        <v>-48427670965.711304</v>
+      </c>
+      <c r="H179" t="s">
+        <v>13</v>
+      </c>
+      <c r="I179">
+        <v>30000</v>
+      </c>
+      <c r="J179">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B180">
+        <v>54382.002118720688</v>
+      </c>
+      <c r="C180">
+        <v>0.5</v>
+      </c>
+      <c r="D180">
+        <v>45518252753.649132</v>
+      </c>
+      <c r="E180" t="s">
+        <v>29</v>
+      </c>
+      <c r="F180">
+        <v>2000</v>
+      </c>
+      <c r="G180">
+        <v>39636729746.925568</v>
+      </c>
+      <c r="H180" t="s">
         <v>9</v>
       </c>
-      <c r="F174">
-        <v>2000</v>
-      </c>
-      <c r="G174">
-        <v>39274548294.962227</v>
-      </c>
-      <c r="H174" t="s">
+      <c r="I180">
+        <v>0</v>
+      </c>
+      <c r="J180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B181">
+        <v>54917.412635528948</v>
+      </c>
+      <c r="C181">
+        <v>0.5</v>
+      </c>
+      <c r="D181">
+        <v>45510200166.581139</v>
+      </c>
+      <c r="E181" t="s">
+        <v>30</v>
+      </c>
+      <c r="F181">
+        <v>2000</v>
+      </c>
+      <c r="G181">
+        <v>38076713308.078041</v>
+      </c>
+      <c r="H181" t="s">
         <v>9</v>
       </c>
-      <c r="I174">
-        <v>30000</v>
-      </c>
-      <c r="J174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B175">
-        <v>68014.663831286598</v>
-      </c>
-      <c r="C175">
-        <v>0.5</v>
-      </c>
-      <c r="D175">
-        <v>45625055534.595047</v>
-      </c>
-      <c r="E175" t="s">
-        <v>28</v>
-      </c>
-      <c r="F175">
-        <v>2000</v>
-      </c>
-      <c r="G175">
-        <v>37656437856.134041</v>
-      </c>
-      <c r="H175" t="s">
+      <c r="I181">
+        <v>0</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="3">
+        <v>92</v>
+      </c>
+      <c r="B182">
+        <v>20141.275508210809</v>
+      </c>
+      <c r="C182">
+        <v>0.5</v>
+      </c>
+      <c r="D182">
+        <v>11538656672.076599</v>
+      </c>
+      <c r="E182" t="s">
+        <v>23</v>
+      </c>
+      <c r="F182">
+        <v>2000</v>
+      </c>
+      <c r="G182">
+        <v>8797459285.4957466</v>
+      </c>
+      <c r="H182" t="s">
+        <v>14</v>
+      </c>
+      <c r="I182">
+        <v>30000</v>
+      </c>
+      <c r="J182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A183" s="3">
+        <v>153</v>
+      </c>
+      <c r="B183">
+        <v>76853.387521036348</v>
+      </c>
+      <c r="C183">
+        <v>0.5</v>
+      </c>
+      <c r="D183">
+        <v>45630534694.182037</v>
+      </c>
+      <c r="E183" t="s">
+        <v>24</v>
+      </c>
+      <c r="F183">
+        <v>2000</v>
+      </c>
+      <c r="G183">
+        <v>-49126963663.181602</v>
+      </c>
+      <c r="H183" t="s">
+        <v>15</v>
+      </c>
+      <c r="I183">
+        <v>30000</v>
+      </c>
+      <c r="J183">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B184">
+        <v>43042.644739441457</v>
+      </c>
+      <c r="C184">
+        <v>0.5</v>
+      </c>
+      <c r="D184">
+        <v>44247974577.88266</v>
+      </c>
+      <c r="E184" t="s">
+        <v>29</v>
+      </c>
+      <c r="F184">
+        <v>2000</v>
+      </c>
+      <c r="G184">
+        <v>-9411492105.435709</v>
+      </c>
+      <c r="H184" t="s">
         <v>9</v>
       </c>
-      <c r="I175">
-        <v>30000</v>
-      </c>
-      <c r="J175">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B176">
-        <v>53903.196729560907</v>
-      </c>
-      <c r="C176">
-        <v>0.5</v>
-      </c>
-      <c r="D176">
-        <v>36152247074.781609</v>
-      </c>
-      <c r="E176" t="s">
-        <v>27</v>
-      </c>
-      <c r="F176">
-        <v>2000</v>
-      </c>
-      <c r="G176">
-        <v>-29941568211.32774</v>
-      </c>
-      <c r="H176" t="s">
+      <c r="I184">
+        <v>0</v>
+      </c>
+      <c r="J184">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B185">
+        <v>43457.153532866891</v>
+      </c>
+      <c r="C185">
+        <v>0.5</v>
+      </c>
+      <c r="D185">
+        <v>44239979220.169907</v>
+      </c>
+      <c r="E185" t="s">
+        <v>31</v>
+      </c>
+      <c r="F185">
+        <v>2000</v>
+      </c>
+      <c r="G185">
+        <v>-10794015052.95153</v>
+      </c>
+      <c r="H185" t="s">
         <v>9</v>
       </c>
-      <c r="I176">
-        <v>0</v>
-      </c>
-      <c r="J176">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="177" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B177">
-        <v>54410.325563740516</v>
-      </c>
-      <c r="C177">
-        <v>0.5</v>
-      </c>
-      <c r="D177">
-        <v>36142898870.665154</v>
-      </c>
-      <c r="E177" t="s">
-        <v>28</v>
-      </c>
-      <c r="F177">
-        <v>2000</v>
-      </c>
-      <c r="G177">
-        <v>-31624764918.147991</v>
-      </c>
-      <c r="H177" t="s">
+      <c r="I185">
+        <v>0</v>
+      </c>
+      <c r="J185">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="3">
+        <v>91</v>
+      </c>
+      <c r="B186">
+        <v>20204.21675520407</v>
+      </c>
+      <c r="C186">
+        <v>0.5</v>
+      </c>
+      <c r="D186">
+        <v>11412353729.80073</v>
+      </c>
+      <c r="E186" t="s">
+        <v>23</v>
+      </c>
+      <c r="F186">
+        <v>2000</v>
+      </c>
+      <c r="G186">
+        <v>8666211435.9383888</v>
+      </c>
+      <c r="H186" t="s">
+        <v>13</v>
+      </c>
+      <c r="I186">
+        <v>30000</v>
+      </c>
+      <c r="J186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A187" s="3">
+        <v>154</v>
+      </c>
+      <c r="B187">
+        <v>77635.159985174396</v>
+      </c>
+      <c r="C187">
+        <v>0.5</v>
+      </c>
+      <c r="D187">
+        <v>45552330647.758202</v>
+      </c>
+      <c r="E187" t="s">
+        <v>24</v>
+      </c>
+      <c r="F187">
+        <v>2000</v>
+      </c>
+      <c r="G187">
+        <v>-50495327938.463402</v>
+      </c>
+      <c r="H187" t="s">
+        <v>16</v>
+      </c>
+      <c r="I187">
+        <v>30000</v>
+      </c>
+      <c r="J187">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B188">
+        <v>41677.977799465807</v>
+      </c>
+      <c r="C188">
+        <v>0.5</v>
+      </c>
+      <c r="D188">
+        <v>43730821878.135834</v>
+      </c>
+      <c r="E188" t="s">
+        <v>36</v>
+      </c>
+      <c r="F188">
+        <v>2000</v>
+      </c>
+      <c r="G188">
+        <v>-8225185760.5144157</v>
+      </c>
+      <c r="H188" t="s">
         <v>9</v>
       </c>
-      <c r="I177">
-        <v>0</v>
-      </c>
-      <c r="J177">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="178" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B178">
-        <v>52316.086802824248</v>
-      </c>
-      <c r="C178">
-        <v>0.5</v>
-      </c>
-      <c r="D178">
-        <v>33833532056.768509</v>
-      </c>
-      <c r="E178" t="s">
-        <v>27</v>
-      </c>
-      <c r="F178">
-        <v>2000</v>
-      </c>
-      <c r="G178">
-        <v>-30318561389.1497</v>
-      </c>
-      <c r="H178" t="s">
+      <c r="I188">
+        <v>0</v>
+      </c>
+      <c r="J188">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B189">
+        <v>42092.121018637619</v>
+      </c>
+      <c r="C189">
+        <v>0.5</v>
+      </c>
+      <c r="D189">
+        <v>43722854609.138153</v>
+      </c>
+      <c r="E189" t="s">
+        <v>37</v>
+      </c>
+      <c r="F189">
+        <v>2000</v>
+      </c>
+      <c r="G189">
+        <v>-9595335458.5274639</v>
+      </c>
+      <c r="H189" t="s">
         <v>9</v>
       </c>
-      <c r="I178">
-        <v>30000</v>
-      </c>
-      <c r="J178">
-        <v>1115970.8999999999</v>
-      </c>
-    </row>
-    <row r="179" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B179">
-        <v>52818.955692821633</v>
-      </c>
-      <c r="C179">
-        <v>0.5</v>
-      </c>
-      <c r="D179">
-        <v>33824347003.661751</v>
-      </c>
-      <c r="E179" t="s">
-        <v>28</v>
-      </c>
-      <c r="F179">
-        <v>2000</v>
-      </c>
-      <c r="G179">
-        <v>-31979931245.781521</v>
-      </c>
-      <c r="H179" t="s">
+      <c r="I189">
+        <v>0</v>
+      </c>
+      <c r="J189">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A190" s="3">
+        <v>155</v>
+      </c>
+      <c r="B190">
+        <v>77972.636944767553</v>
+      </c>
+      <c r="C190">
+        <v>0.5</v>
+      </c>
+      <c r="D190">
+        <v>45517080550.665993</v>
+      </c>
+      <c r="E190" t="s">
+        <v>24</v>
+      </c>
+      <c r="F190">
+        <v>2000</v>
+      </c>
+      <c r="G190">
+        <v>-50954555487.650848</v>
+      </c>
+      <c r="H190" t="s">
+        <v>17</v>
+      </c>
+      <c r="I190">
+        <v>30000</v>
+      </c>
+      <c r="J190">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A191" s="3">
+        <v>156</v>
+      </c>
+      <c r="B191">
+        <v>80292.148994584961</v>
+      </c>
+      <c r="C191">
+        <v>0.5</v>
+      </c>
+      <c r="D191">
+        <v>45500943700.806664</v>
+      </c>
+      <c r="E191" t="s">
+        <v>24</v>
+      </c>
+      <c r="F191">
+        <v>2000</v>
+      </c>
+      <c r="G191">
+        <v>-53658207844.543114</v>
+      </c>
+      <c r="H191" t="s">
+        <v>18</v>
+      </c>
+      <c r="I191">
+        <v>30000</v>
+      </c>
+      <c r="J191">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B192">
+        <v>48120.651527216673</v>
+      </c>
+      <c r="C192">
+        <v>0.5</v>
+      </c>
+      <c r="D192">
+        <v>45068715192.022537</v>
+      </c>
+      <c r="E192" t="s">
+        <v>36</v>
+      </c>
+      <c r="F192">
+        <v>2000</v>
+      </c>
+      <c r="G192">
+        <v>39761732291.408417</v>
+      </c>
+      <c r="H192" t="s">
         <v>9</v>
       </c>
-      <c r="I179">
-        <v>30000</v>
-      </c>
-      <c r="J179">
+      <c r="I192">
+        <v>0</v>
+      </c>
+      <c r="J192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B193">
+        <v>48679.513965852733</v>
+      </c>
+      <c r="C193">
+        <v>0.5</v>
+      </c>
+      <c r="D193">
+        <v>45060607029.715057</v>
+      </c>
+      <c r="E193" t="s">
+        <v>37</v>
+      </c>
+      <c r="F193">
+        <v>2000</v>
+      </c>
+      <c r="G193">
+        <v>38204754227.615646</v>
+      </c>
+      <c r="H193" t="s">
+        <v>9</v>
+      </c>
+      <c r="I193">
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="3">
+        <v>98</v>
+      </c>
+      <c r="B194">
+        <v>23352.711087550659</v>
+      </c>
+      <c r="C194">
+        <v>0.5</v>
+      </c>
+      <c r="D194">
+        <v>11411382815.65556</v>
+      </c>
+      <c r="E194" t="s">
+        <v>23</v>
+      </c>
+      <c r="F194">
+        <v>2000</v>
+      </c>
+      <c r="G194">
+        <v>8520063240.3933992</v>
+      </c>
+      <c r="H194" t="s">
+        <v>20</v>
+      </c>
+      <c r="I194">
+        <v>30000</v>
+      </c>
+      <c r="J194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="3">
+        <v>99</v>
+      </c>
+      <c r="B195">
+        <v>25790.727244949579</v>
+      </c>
+      <c r="C195">
+        <v>0.5</v>
+      </c>
+      <c r="D195">
+        <v>11411109391.88575</v>
+      </c>
+      <c r="E195" t="s">
+        <v>23</v>
+      </c>
+      <c r="F195">
+        <v>2000</v>
+      </c>
+      <c r="G195">
+        <v>8465090000.3280087</v>
+      </c>
+      <c r="H195" t="s">
+        <v>21</v>
+      </c>
+      <c r="I195">
+        <v>30000</v>
+      </c>
+      <c r="J195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B196">
+        <v>22089.563463968079</v>
+      </c>
+      <c r="C196">
+        <v>0.5</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196" t="s">
+        <v>39</v>
+      </c>
+      <c r="F196">
+        <v>2000</v>
+      </c>
+      <c r="G196" s="4">
+        <v>-2332529839.0764298</v>
+      </c>
+      <c r="H196" t="s">
+        <v>9</v>
+      </c>
+      <c r="I196">
+        <v>0</v>
+      </c>
+      <c r="J196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B197">
+        <v>22444.799538309151</v>
+      </c>
+      <c r="C197">
+        <v>0.5</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197" t="s">
+        <v>40</v>
+      </c>
+      <c r="F197">
+        <v>2000</v>
+      </c>
+      <c r="G197" s="4">
+        <v>-3104218115.3621211</v>
+      </c>
+      <c r="H197" t="s">
+        <v>9</v>
+      </c>
+      <c r="I197">
+        <v>0</v>
+      </c>
+      <c r="J197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B198">
+        <v>23786.412796295652</v>
+      </c>
+      <c r="C198">
+        <v>0.5</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198" t="s">
+        <v>41</v>
+      </c>
+      <c r="F198">
+        <v>2000</v>
+      </c>
+      <c r="G198" s="4">
+        <v>-2373274113.2180471</v>
+      </c>
+      <c r="H198" t="s">
+        <v>9</v>
+      </c>
+      <c r="I198">
+        <v>30000</v>
+      </c>
+      <c r="J198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B199">
+        <v>24161.102904664702</v>
+      </c>
+      <c r="C199">
+        <v>0.5</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199" t="s">
+        <v>40</v>
+      </c>
+      <c r="F199">
+        <v>2000</v>
+      </c>
+      <c r="G199" s="4">
+        <v>-3180384352.007998</v>
+      </c>
+      <c r="H199" t="s">
+        <v>9</v>
+      </c>
+      <c r="I199">
+        <v>30000</v>
+      </c>
+      <c r="J199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A200" s="3">
+        <v>150</v>
+      </c>
+      <c r="B200">
+        <v>82759.777568824735</v>
+      </c>
+      <c r="C200">
+        <v>0.5</v>
+      </c>
+      <c r="D200">
+        <v>45624202826.455658</v>
+      </c>
+      <c r="E200" t="s">
+        <v>24</v>
+      </c>
+      <c r="F200">
+        <v>2000</v>
+      </c>
+      <c r="G200">
+        <v>-55809608702.400337</v>
+      </c>
+      <c r="H200" t="s">
+        <v>12</v>
+      </c>
+      <c r="I200">
+        <v>30000</v>
+      </c>
+      <c r="J200">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A201" s="3">
+        <v>157</v>
+      </c>
+      <c r="B201">
+        <v>84501.197139652882</v>
+      </c>
+      <c r="C201">
+        <v>0.5</v>
+      </c>
+      <c r="D201">
+        <v>45611555088.877579</v>
+      </c>
+      <c r="E201" t="s">
+        <v>24</v>
+      </c>
+      <c r="F201">
+        <v>2000</v>
+      </c>
+      <c r="G201">
+        <v>-57856332261.281601</v>
+      </c>
+      <c r="H201" t="s">
+        <v>19</v>
+      </c>
+      <c r="I201">
+        <v>30000</v>
+      </c>
+      <c r="J201">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A202" s="3">
+        <v>158</v>
+      </c>
+      <c r="B202">
+        <v>89519.889499620855</v>
+      </c>
+      <c r="C202">
+        <v>0.5</v>
+      </c>
+      <c r="D202">
+        <v>45692079294.099579</v>
+      </c>
+      <c r="E202" t="s">
+        <v>24</v>
+      </c>
+      <c r="F202">
+        <v>2000</v>
+      </c>
+      <c r="G202">
+        <v>-63012463750.982613</v>
+      </c>
+      <c r="H202" t="s">
+        <v>20</v>
+      </c>
+      <c r="I202">
+        <v>30000</v>
+      </c>
+      <c r="J202">
+        <v>1115970.8999999999</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A203" s="3">
+        <v>159</v>
+      </c>
+      <c r="B203">
+        <v>104513.00660286591</v>
+      </c>
+      <c r="C203">
+        <v>0.5</v>
+      </c>
+      <c r="D203">
+        <v>45691116442.457909</v>
+      </c>
+      <c r="E203" t="s">
+        <v>24</v>
+      </c>
+      <c r="F203">
+        <v>2000</v>
+      </c>
+      <c r="G203">
+        <v>-79806248476.391983</v>
+      </c>
+      <c r="H203" t="s">
+        <v>21</v>
+      </c>
+      <c r="I203">
+        <v>30000</v>
+      </c>
+      <c r="J203">
         <v>1115970.8999999999</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J171" xr:uid="{C3F4E1A5-BCB4-DA4F-80B4-79B6563091D1}">
+  <autoFilter ref="A1:J203" xr:uid="{C3F4E1A5-BCB4-DA4F-80B4-79B6563091D1}">
     <filterColumn colId="8">
       <filters>
         <filter val="30000"/>
@@ -6202,8 +6966,8 @@
         <filter val="1115970.9"/>
       </filters>
     </filterColumn>
-    <sortState ref="A4:J171">
-      <sortCondition descending="1" ref="G1:G171"/>
+    <sortState ref="A5:J203">
+      <sortCondition ref="B1:B203"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>